<commit_message>
Finish the first stage of Literature Review
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5F4A3B-AA16-CD40-8327-25EAA464F716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F192A570-853F-664B-9F60-364C2155F495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="22980" windowHeight="15880" activeTab="1" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
+    <workbookView xWindow="160" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
   <sheets>
     <sheet name="Four-phase flow diagram" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
   <si>
     <t>Google Scholar</t>
   </si>
@@ -91,51 +91,6 @@
   </si>
   <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Literature Review</t>
-  </si>
-  <si>
-    <t>Qualitative</t>
-  </si>
-  <si>
-    <t>Analysis</t>
-  </si>
-  <si>
-    <t>Quantitative</t>
-  </si>
-  <si>
-    <t>Experiment</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>Simulation</t>
-  </si>
-  <si>
-    <t>Survey</t>
-  </si>
-  <si>
-    <t>Field study</t>
-  </si>
-  <si>
-    <t>Agent-based modeling</t>
-  </si>
-  <si>
-    <t>Quantiative</t>
-  </si>
-  <si>
-    <t>Analytics</t>
-  </si>
-  <si>
-    <t>Simulation/Experiment</t>
-  </si>
-  <si>
-    <t>Theoretical work</t>
-  </si>
-  <si>
-    <t>empirical + model</t>
   </si>
   <si>
     <t>Additional records identified through other sources</t>
@@ -393,9 +348,6 @@
     </r>
   </si>
   <si>
-    <t>Pilot study</t>
-  </si>
-  <si>
     <t>"Optimal Power Flow" "Reinforcement Learning"</t>
   </si>
   <si>
@@ -502,6 +454,117 @@
   </si>
   <si>
     <t>Optimal Operable Power Flow: Sample-Efficient Holomorphic Embedding-Based Reinforcement Learning</t>
+  </si>
+  <si>
+    <t>"safe reinforcement learning" "optimal power flow" "EV"</t>
+  </si>
+  <si>
+    <t>Rule-based shields embedded safe reinforcement learning approach for electric vehicle charging control</t>
+  </si>
+  <si>
+    <t>Guan et al.</t>
+  </si>
+  <si>
+    <t>International Journal of Electrical Power and Energy Systems</t>
+  </si>
+  <si>
+    <t>Not directly related to OPF. Only focus on EV charging and discharing decisions</t>
+  </si>
+  <si>
+    <t>Real-Time Sequential Security-Constrained Optimal Power Flow: A Hybrid Knowledge-Data-Driven Reinforcement Learning Approach</t>
+  </si>
+  <si>
+    <t>Yi et al.</t>
+  </si>
+  <si>
+    <t>Safety layer</t>
+  </si>
+  <si>
+    <t>Research and Application of Safe Reinforcement Learning in Power System</t>
+  </si>
+  <si>
+    <t>2023 8th Asia Conference on Power and Electrical Engineering</t>
+  </si>
+  <si>
+    <t>SRL, concept explanation, application introduction</t>
+  </si>
+  <si>
+    <t>Ye et al.</t>
+  </si>
+  <si>
+    <t>Safe Deep Reinforcement Learning for Microgrid Energy Management in Distribution Networks With Leveraged Spatial–Temporal Perception</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Smart Grid</t>
+  </si>
+  <si>
+    <t>SRL, interior-point policy optimization</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning with Enhanced Safety for Optimal Dispatch of Distributed Energy Resources in Active Distribution Networks</t>
+  </si>
+  <si>
+    <t>Yang et al.</t>
+  </si>
+  <si>
+    <t>Safe Reinforcement Learning for Energy Management of Electrified Vehicle with Novel Physics-Informed Exploration Strategy</t>
+  </si>
+  <si>
+    <t>Biswas et al.</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Transportation Electrification</t>
+  </si>
+  <si>
+    <t>SRL, advisor</t>
+  </si>
+  <si>
+    <t>Not OPF, SRL</t>
+  </si>
+  <si>
+    <t>Improved Proximal Policy Optimization Algorithm for Sequential Security-constrained Optimal Power Flow Based on Expert Knowledge and Safety Layer</t>
+  </si>
+  <si>
+    <t>Chen et al.</t>
+  </si>
+  <si>
+    <t>SRL, safety layer, expert</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning for Selective Key Applications in Power Systems: Recent Advances and Future Challenges</t>
+  </si>
+  <si>
+    <t>RL in power system review (focus on the algorithm)</t>
+  </si>
+  <si>
+    <t>Model-Free Economic Dispatch for Virtual Power Plants: An Adversarial Safe Reinforcement Learning Approach</t>
+  </si>
+  <si>
+    <t>SRL, voltage violation missing, still uses penalty</t>
+  </si>
+  <si>
+    <t>Learning the Optimal Power Flow: Environment Design Matters</t>
+  </si>
+  <si>
+    <t>Wolgast and Nieße</t>
+  </si>
+  <si>
+    <t>Environment design tips</t>
+  </si>
+  <si>
+    <t>Reinforcement Learning Techniques for Optimal Power Control in Grid-Connected Microgrids: A Comprehensive Review</t>
+  </si>
+  <si>
+    <t>Arwa and Folly</t>
+  </si>
+  <si>
+    <t>IEEE Access</t>
+  </si>
+  <si>
+    <t>Navigating the Landscape of Deep Reinforcement Learning for Power System Stability Control: A Review</t>
+  </si>
+  <si>
+    <t>Massaoudi et al.</t>
   </si>
 </sst>
 </file>
@@ -768,7 +831,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -839,6 +902,45 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -853,9 +955,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -872,51 +971,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -965,21 +1029,21 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color theme="5"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2293,22 +2357,22 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+        <v>23</v>
+      </c>
+      <c r="F2" s="30"/>
+      <c r="G2" s="31"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="49"/>
+      <c r="K2" s="33"/>
       <c r="L2" s="1"/>
       <c r="M2" s="29" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42"/>
+        <v>32</v>
+      </c>
+      <c r="N2" s="30"/>
+      <c r="O2" s="31"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="49"/>
+      <c r="Q2" s="33"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2337,19 +2401,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="49"/>
-      <c r="G3" s="50"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="35"/>
+      <c r="K3" s="38"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="48"/>
-      <c r="N3" s="49"/>
-      <c r="O3" s="50"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="34"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="35"/>
+      <c r="Q3" s="38"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2378,19 +2442,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="45"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="35"/>
+      <c r="K4" s="38"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="44"/>
-      <c r="O4" s="45"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="37"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="35"/>
+      <c r="Q4" s="38"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -2541,15 +2605,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="39" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="51" t="s">
-        <v>42</v>
+      <c r="F8" s="39" t="s">
+        <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="41" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -2588,11 +2652,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="52"/>
+      <c r="D9" s="40"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="52"/>
+      <c r="F9" s="40"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="54"/>
+      <c r="H9" s="42"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -2715,18 +2779,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="36" t="s">
-        <v>43</v>
-      </c>
-      <c r="I12" s="37"/>
-      <c r="J12" s="38"/>
+      <c r="H12" s="48" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="49"/>
+      <c r="J12" s="50"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="36" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="39"/>
-      <c r="O12" s="40"/>
+      <c r="M12" s="48" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="51"/>
+      <c r="O12" s="52"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2842,18 +2906,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="36" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="37"/>
-      <c r="J15" s="38"/>
+      <c r="H15" s="48" t="s">
+        <v>29</v>
+      </c>
+      <c r="I15" s="49"/>
+      <c r="J15" s="50"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="N15" s="37"/>
-      <c r="O15" s="38"/>
+      <c r="M15" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="N15" s="49"/>
+      <c r="O15" s="50"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -2970,17 +3034,17 @@
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
+        <v>18</v>
+      </c>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="N18" s="30"/>
-      <c r="O18" s="31"/>
+        <v>25</v>
+      </c>
+      <c r="N18" s="43"/>
+      <c r="O18" s="44"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3014,14 +3078,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="45"/>
+      <c r="H19" s="35"/>
+      <c r="I19" s="36"/>
+      <c r="J19" s="37"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="32"/>
-      <c r="N19" s="33"/>
-      <c r="O19" s="34"/>
+      <c r="M19" s="45"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="47"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3138,10 +3202,10 @@
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="29" t="s">
-        <v>41</v>
-      </c>
-      <c r="I22" s="30"/>
-      <c r="J22" s="31"/>
+        <v>26</v>
+      </c>
+      <c r="I22" s="43"/>
+      <c r="J22" s="44"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3180,9 +3244,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="32"/>
-      <c r="I23" s="33"/>
-      <c r="J23" s="34"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="47"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3261,13 +3325,13 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="46" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="47"/>
+      <c r="G25" s="53" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="54"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -3385,8 +3449,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -3916,13 +3980,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="M2:O4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H22:J23"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="H12:J12"/>
@@ -3932,6 +3989,13 @@
     <mergeCell ref="H18:J19"/>
     <mergeCell ref="M18:O19"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E2:G4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:O4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3944,14 +4008,14 @@
   <dimension ref="A1:T346"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="D6" sqref="D6:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="4.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="44.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="87.6640625" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.5" style="2" customWidth="1"/>
@@ -4007,7 +4071,7 @@
       <c r="K2" s="55"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="N2" s="8"/>
       <c r="O2" s="20" t="s">
@@ -4039,7 +4103,7 @@
       <c r="M3" s="8"/>
       <c r="N3" s="6"/>
       <c r="O3" s="23" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="P3" s="12"/>
       <c r="Q3" s="9"/>
@@ -4102,13 +4166,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F6" s="14" t="s">
         <v>4</v>
@@ -4136,13 +4200,13 @@
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F7" s="8">
         <v>2020</v>
@@ -4159,12 +4223,8 @@
       <c r="L7" s="8"/>
       <c r="M7" s="6"/>
       <c r="N7" s="8"/>
-      <c r="O7" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O7" s="8"/>
+      <c r="P7" s="12"/>
       <c r="Q7" s="28"/>
       <c r="R7" s="9"/>
       <c r="S7" s="9"/>
@@ -4176,13 +4236,13 @@
         <v>2</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F8" s="8">
         <v>2020</v>
@@ -4199,12 +4259,8 @@
       <c r="L8" s="8"/>
       <c r="M8" s="6"/>
       <c r="N8" s="8"/>
-      <c r="O8" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P8" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O8" s="8"/>
+      <c r="P8" s="12"/>
       <c r="Q8" s="28"/>
       <c r="R8" s="9"/>
       <c r="S8" s="9"/>
@@ -4216,13 +4272,13 @@
         <v>3</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F9" s="8">
         <v>2021</v>
@@ -4252,13 +4308,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="F10" s="8">
         <v>2022</v>
@@ -4275,12 +4331,8 @@
       <c r="L10" s="8"/>
       <c r="M10" s="6"/>
       <c r="N10" s="8"/>
-      <c r="O10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O10" s="8"/>
+      <c r="P10" s="12"/>
       <c r="Q10" s="28"/>
       <c r="R10" s="9"/>
       <c r="S10" s="9"/>
@@ -4292,13 +4344,13 @@
         <v>5</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>60</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="F11" s="8">
         <v>2022</v>
@@ -4328,13 +4380,13 @@
         <v>6</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="F12" s="8">
         <v>2022</v>
@@ -4351,12 +4403,8 @@
       <c r="L12" s="8"/>
       <c r="M12" s="6"/>
       <c r="N12" s="8"/>
-      <c r="O12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O12" s="8"/>
+      <c r="P12" s="12"/>
       <c r="Q12" s="28"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
@@ -4368,13 +4416,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F13" s="8">
         <v>2023</v>
@@ -4391,12 +4439,8 @@
       <c r="L13" s="8"/>
       <c r="M13" s="6"/>
       <c r="N13" s="8"/>
-      <c r="O13" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="12"/>
       <c r="Q13" s="28"/>
       <c r="R13" s="9"/>
       <c r="S13" s="9"/>
@@ -4408,13 +4452,13 @@
         <v>8</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>66</v>
+        <v>50</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>73</v>
+        <v>57</v>
       </c>
       <c r="F14" s="8">
         <v>2024</v>
@@ -4431,12 +4475,8 @@
       <c r="L14" s="8"/>
       <c r="M14" s="6"/>
       <c r="N14" s="8"/>
-      <c r="O14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P14" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O14" s="8"/>
+      <c r="P14" s="12"/>
       <c r="Q14" s="28"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
@@ -4448,13 +4488,13 @@
         <v>9</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>67</v>
+        <v>51</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F15" s="8">
         <v>2024</v>
@@ -4471,12 +4511,8 @@
       <c r="L15" s="8"/>
       <c r="M15" s="6"/>
       <c r="N15" s="8"/>
-      <c r="O15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P15" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O15" s="8"/>
+      <c r="P15" s="12"/>
       <c r="Q15" s="28"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
@@ -4488,13 +4524,13 @@
         <v>10</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>77</v>
+        <v>61</v>
       </c>
       <c r="F16" s="8">
         <v>2022</v>
@@ -4511,12 +4547,8 @@
       <c r="L16" s="8"/>
       <c r="M16" s="6"/>
       <c r="N16" s="8"/>
-      <c r="O16" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P16" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O16" s="8"/>
+      <c r="P16" s="12"/>
       <c r="Q16" s="28"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
@@ -4528,13 +4560,13 @@
         <v>11</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>71</v>
+        <v>55</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F17" s="8">
         <v>2024</v>
@@ -4551,12 +4583,8 @@
       <c r="L17" s="8"/>
       <c r="M17" s="6"/>
       <c r="N17" s="8"/>
-      <c r="O17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P17" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O17" s="8"/>
+      <c r="P17" s="12"/>
       <c r="Q17" s="28"/>
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
@@ -4568,13 +4596,13 @@
         <v>12</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>78</v>
+        <v>62</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>80</v>
+        <v>64</v>
       </c>
       <c r="F18" s="8">
         <v>2020</v>
@@ -4591,12 +4619,8 @@
       <c r="L18" s="8"/>
       <c r="M18" s="6"/>
       <c r="N18" s="8"/>
-      <c r="O18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P18" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O18" s="8"/>
+      <c r="P18" s="12"/>
       <c r="Q18" s="28"/>
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
@@ -4608,13 +4632,13 @@
         <v>13</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>81</v>
+        <v>65</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F19" s="8">
         <v>2020</v>
@@ -4631,12 +4655,8 @@
       <c r="L19" s="8"/>
       <c r="M19" s="6"/>
       <c r="N19" s="8"/>
-      <c r="O19" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P19" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O19" s="8"/>
+      <c r="P19" s="12"/>
       <c r="Q19" s="28"/>
       <c r="R19" s="9"/>
       <c r="S19" s="9"/>
@@ -4648,13 +4668,13 @@
         <v>14</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="F20" s="8">
         <v>2024</v>
@@ -4671,12 +4691,8 @@
       <c r="L20" s="8"/>
       <c r="M20" s="6"/>
       <c r="N20" s="8"/>
-      <c r="O20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="P20" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O20" s="8"/>
+      <c r="P20" s="12"/>
       <c r="Q20" s="28"/>
       <c r="R20" s="9"/>
       <c r="S20" s="9"/>
@@ -4684,9 +4700,7 @@
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="6"/>
-      <c r="B21" s="12">
-        <v>15</v>
-      </c>
+      <c r="B21" s="12"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -4708,9 +4722,7 @@
     </row>
     <row r="22" spans="1:20">
       <c r="A22" s="6"/>
-      <c r="B22" s="12">
-        <v>16</v>
-      </c>
+      <c r="B22" s="12"/>
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
@@ -4718,12 +4730,15 @@
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
+      <c r="J22" s="8">
+        <v>13</v>
+      </c>
+      <c r="K22" s="8">
+        <v>1</v>
+      </c>
       <c r="L22" s="8"/>
       <c r="M22" s="6"/>
       <c r="N22" s="8"/>
-      <c r="O22" s="8"/>
       <c r="P22" s="12"/>
       <c r="Q22" s="28"/>
       <c r="R22" s="9"/>
@@ -4732,9 +4747,7 @@
     </row>
     <row r="23" spans="1:20">
       <c r="A23" s="6"/>
-      <c r="B23" s="12">
-        <v>17</v>
-      </c>
+      <c r="B23" s="12"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
@@ -4757,9 +4770,11 @@
     <row r="24" spans="1:20">
       <c r="A24" s="6"/>
       <c r="B24" s="12">
-        <v>18</v>
-      </c>
-      <c r="C24" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>69</v>
+      </c>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
       <c r="F24" s="8"/>
@@ -4771,40 +4786,48 @@
       <c r="L24" s="8"/>
       <c r="M24" s="6"/>
       <c r="N24" s="8"/>
-      <c r="O24" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="P24" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="O24" s="8"/>
+      <c r="P24" s="12"/>
       <c r="Q24" s="28"/>
-      <c r="R24" s="9"/>
+      <c r="R24" s="9">
+        <v>598</v>
+      </c>
       <c r="S24" s="9"/>
       <c r="T24" s="9"/>
     </row>
     <row r="25" spans="1:20">
       <c r="A25" s="6"/>
       <c r="B25" s="12">
-        <v>19</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="8"/>
+        <v>15</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="8">
+        <v>2024</v>
+      </c>
       <c r="G25" s="8"/>
-      <c r="H25" s="8"/>
+      <c r="H25" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
-      <c r="M25" s="6"/>
+      <c r="M25" s="6" t="s">
+        <v>73</v>
+      </c>
       <c r="N25" s="8"/>
-      <c r="O25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P25" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="O25" s="8"/>
+      <c r="P25" s="12"/>
       <c r="Q25" s="28"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
@@ -4813,26 +4836,36 @@
     <row r="26" spans="1:20">
       <c r="A26" s="6"/>
       <c r="B26" s="12">
-        <v>20</v>
-      </c>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F26" s="8">
+        <v>2024</v>
+      </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="8"/>
+      <c r="H26" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
+      <c r="J26" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K26" s="8"/>
       <c r="L26" s="8"/>
-      <c r="M26" s="6"/>
+      <c r="M26" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="N26" s="8"/>
-      <c r="O26" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P26" s="12" t="s">
-        <v>24</v>
-      </c>
+      <c r="O26" s="8"/>
+      <c r="P26" s="12"/>
       <c r="Q26" s="28"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
@@ -4840,23 +4873,36 @@
     </row>
     <row r="27" spans="1:20">
       <c r="A27" s="6"/>
-      <c r="B27" s="12"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="8"/>
+      <c r="B27" s="12">
+        <v>17</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="F27" s="8">
+        <v>2023</v>
+      </c>
       <c r="G27" s="8"/>
-      <c r="H27" s="8"/>
+      <c r="H27" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I27" s="8"/>
-      <c r="J27" s="8">
-        <v>13</v>
-      </c>
-      <c r="K27" s="8">
-        <v>1</v>
-      </c>
+      <c r="J27" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K27" s="8"/>
       <c r="L27" s="8"/>
-      <c r="M27" s="6"/>
+      <c r="M27" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="N27" s="8"/>
+      <c r="O27" s="8"/>
       <c r="P27" s="12"/>
       <c r="Q27" s="28"/>
       <c r="R27" s="9"/>
@@ -4865,18 +4911,34 @@
     </row>
     <row r="28" spans="1:20">
       <c r="A28" s="6"/>
-      <c r="B28" s="12"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="8"/>
+      <c r="B28" s="12">
+        <v>18</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" s="8">
+        <v>2023</v>
+      </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="8"/>
+      <c r="H28" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
-      <c r="M28" s="6"/>
+      <c r="M28" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="N28" s="8"/>
       <c r="O28" s="8"/>
       <c r="P28" s="12"/>
@@ -4888,52 +4950,74 @@
     <row r="29" spans="1:20">
       <c r="A29" s="6"/>
       <c r="B29" s="12">
-        <v>5</v>
-      </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="6"/>
-      <c r="F29" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="8">
+        <v>2024</v>
+      </c>
       <c r="G29" s="8"/>
-      <c r="H29" s="8"/>
+      <c r="H29" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
+      <c r="J29" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K29" s="8"/>
       <c r="L29" s="8"/>
-      <c r="M29" s="6"/>
+      <c r="M29" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="N29" s="8"/>
       <c r="O29" s="8"/>
       <c r="P29" s="12"/>
       <c r="Q29" s="28"/>
-      <c r="R29" s="9">
-        <v>598</v>
-      </c>
+      <c r="R29" s="9"/>
       <c r="S29" s="9"/>
       <c r="T29" s="9"/>
     </row>
     <row r="30" spans="1:20">
       <c r="A30" s="6"/>
       <c r="B30" s="12">
-        <v>21</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="8">
+        <v>2024</v>
+      </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="8"/>
+      <c r="H30" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
+      <c r="J30" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K30" s="8"/>
       <c r="L30" s="8"/>
-      <c r="M30" s="6"/>
+      <c r="M30" s="6" t="s">
+        <v>90</v>
+      </c>
       <c r="N30" s="8"/>
-      <c r="O30" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O30" s="8"/>
+      <c r="P30" s="12"/>
       <c r="Q30" s="28"/>
       <c r="R30" s="9"/>
       <c r="S30" s="9"/>
@@ -4942,26 +5026,36 @@
     <row r="31" spans="1:20">
       <c r="A31" s="6"/>
       <c r="B31" s="12">
-        <v>22</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="8">
+        <v>2024</v>
+      </c>
       <c r="G31" s="8"/>
-      <c r="H31" s="8"/>
+      <c r="H31" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K31" s="8"/>
       <c r="L31" s="8"/>
-      <c r="M31" s="6"/>
+      <c r="M31" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="N31" s="8"/>
-      <c r="O31" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P31" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O31" s="8"/>
+      <c r="P31" s="12"/>
       <c r="Q31" s="28"/>
       <c r="R31" s="9"/>
       <c r="S31" s="9"/>
@@ -4970,26 +5064,36 @@
     <row r="32" spans="1:20">
       <c r="A32" s="6"/>
       <c r="B32" s="12">
-        <v>23</v>
-      </c>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F32" s="8">
+        <v>2022</v>
+      </c>
       <c r="G32" s="8"/>
-      <c r="H32" s="8"/>
+      <c r="H32" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
+      <c r="J32" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K32" s="8"/>
       <c r="L32" s="8"/>
-      <c r="M32" s="6"/>
+      <c r="M32" s="6" t="s">
+        <v>95</v>
+      </c>
       <c r="N32" s="8"/>
-      <c r="O32" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P32" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O32" s="8"/>
+      <c r="P32" s="12"/>
       <c r="Q32" s="28"/>
       <c r="R32" s="9"/>
       <c r="S32" s="9"/>
@@ -4998,26 +5102,36 @@
     <row r="33" spans="1:20">
       <c r="A33" s="6"/>
       <c r="B33" s="12">
-        <v>24</v>
-      </c>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="F33" s="8">
+        <v>2024</v>
+      </c>
       <c r="G33" s="8"/>
-      <c r="H33" s="8"/>
+      <c r="H33" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
+      <c r="J33" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K33" s="8"/>
       <c r="L33" s="8"/>
-      <c r="M33" s="6"/>
+      <c r="M33" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="N33" s="8"/>
-      <c r="O33" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P33" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O33" s="8"/>
+      <c r="P33" s="12"/>
       <c r="Q33" s="28"/>
       <c r="R33" s="9"/>
       <c r="S33" s="9"/>
@@ -5025,9 +5139,7 @@
     </row>
     <row r="34" spans="1:20">
       <c r="A34" s="6"/>
-      <c r="B34" s="12">
-        <v>25</v>
-      </c>
+      <c r="B34" s="12"/>
       <c r="C34" s="6"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -5040,12 +5152,8 @@
       <c r="L34" s="8"/>
       <c r="M34" s="6"/>
       <c r="N34" s="8"/>
-      <c r="O34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P34" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O34" s="8"/>
+      <c r="P34" s="12"/>
       <c r="Q34" s="28"/>
       <c r="R34" s="9"/>
       <c r="S34" s="9"/>
@@ -5062,7 +5170,7 @@
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
       <c r="J35" s="8">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K35" s="8">
         <v>0</v>
@@ -5142,12 +5250,8 @@
       <c r="L38" s="8"/>
       <c r="M38" s="6"/>
       <c r="N38" s="8"/>
-      <c r="O38" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P38" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O38" s="8"/>
+      <c r="P38" s="12"/>
       <c r="Q38" s="28"/>
       <c r="R38" s="9"/>
       <c r="S38" s="9"/>
@@ -5169,12 +5273,8 @@
       <c r="L39" s="8"/>
       <c r="M39" s="6"/>
       <c r="N39" s="8"/>
-      <c r="O39" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="P39" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O39" s="8"/>
+      <c r="P39" s="12"/>
       <c r="Q39" s="28"/>
       <c r="R39" s="9"/>
       <c r="S39" s="9"/>
@@ -5295,12 +5395,8 @@
       <c r="L44" s="8"/>
       <c r="M44" s="6"/>
       <c r="N44" s="8"/>
-      <c r="O44" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P44" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O44" s="8"/>
+      <c r="P44" s="12"/>
       <c r="Q44" s="28"/>
       <c r="R44" s="9"/>
       <c r="S44" s="9"/>
@@ -5323,12 +5419,8 @@
       <c r="L45" s="8"/>
       <c r="M45" s="6"/>
       <c r="N45" s="8"/>
-      <c r="O45" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P45" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O45" s="8"/>
+      <c r="P45" s="12"/>
       <c r="Q45" s="28"/>
       <c r="R45" s="9"/>
       <c r="S45" s="9"/>
@@ -5448,9 +5540,7 @@
       <c r="L50" s="8"/>
       <c r="M50" s="6"/>
       <c r="N50" s="8"/>
-      <c r="O50" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="O50" s="8"/>
       <c r="P50" s="12"/>
       <c r="Q50" s="28"/>
       <c r="R50" s="9"/>
@@ -5473,12 +5563,8 @@
       <c r="L51" s="8"/>
       <c r="M51" s="6"/>
       <c r="N51" s="8"/>
-      <c r="O51" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P51" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O51" s="8"/>
+      <c r="P51" s="12"/>
       <c r="Q51" s="28"/>
       <c r="R51" s="9"/>
       <c r="S51" s="9"/>
@@ -5500,12 +5586,8 @@
       <c r="L52" s="8"/>
       <c r="M52" s="6"/>
       <c r="N52" s="8"/>
-      <c r="O52" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P52" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O52" s="8"/>
+      <c r="P52" s="12"/>
       <c r="Q52" s="28"/>
       <c r="R52" s="9"/>
       <c r="S52" s="9"/>
@@ -5527,12 +5609,8 @@
       <c r="L53" s="8"/>
       <c r="M53" s="6"/>
       <c r="N53" s="8"/>
-      <c r="O53" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P53" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O53" s="8"/>
+      <c r="P53" s="12"/>
       <c r="Q53" s="28"/>
       <c r="R53" s="9"/>
       <c r="S53" s="9"/>
@@ -5554,12 +5632,8 @@
       <c r="L54" s="8"/>
       <c r="M54" s="6"/>
       <c r="N54" s="8"/>
-      <c r="O54" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="P54" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O54" s="8"/>
+      <c r="P54" s="12"/>
       <c r="Q54" s="28"/>
       <c r="R54" s="9"/>
       <c r="S54" s="9"/>
@@ -5581,12 +5655,8 @@
       <c r="L55" s="8"/>
       <c r="M55" s="6"/>
       <c r="N55" s="8"/>
-      <c r="O55" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="P55" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O55" s="8"/>
+      <c r="P55" s="12"/>
       <c r="Q55" s="28"/>
       <c r="R55" s="9"/>
       <c r="S55" s="9"/>
@@ -5641,12 +5711,8 @@
       <c r="H59" s="8"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
-      <c r="O59" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="P59" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O59" s="8"/>
+      <c r="P59" s="12"/>
       <c r="Q59" s="28"/>
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
@@ -5663,12 +5729,8 @@
       <c r="H60" s="8"/>
       <c r="J60" s="8"/>
       <c r="K60" s="8"/>
-      <c r="O60" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P60" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O60" s="8"/>
+      <c r="P60" s="12"/>
       <c r="Q60" s="28"/>
       <c r="R60" s="9"/>
       <c r="S60" s="9"/>
@@ -5686,12 +5748,8 @@
       <c r="H61" s="8"/>
       <c r="J61" s="8"/>
       <c r="K61" s="8"/>
-      <c r="O61" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P61" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O61" s="8"/>
+      <c r="P61" s="12"/>
       <c r="Q61" s="28"/>
       <c r="R61" s="9"/>
       <c r="S61" s="9"/>
@@ -5714,9 +5772,7 @@
       <c r="L62" s="8"/>
       <c r="M62" s="6"/>
       <c r="N62" s="8"/>
-      <c r="O62" s="8" t="s">
-        <v>18</v>
-      </c>
+      <c r="O62" s="8"/>
       <c r="P62" s="12"/>
       <c r="Q62" s="28"/>
       <c r="R62" s="9"/>
@@ -5740,12 +5796,8 @@
       <c r="L63" s="8"/>
       <c r="M63" s="6"/>
       <c r="N63" s="8"/>
-      <c r="O63" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="P63" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O63" s="8"/>
+      <c r="P63" s="12"/>
       <c r="Q63" s="28"/>
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
@@ -5774,15 +5826,15 @@
     <row r="66" spans="1:20" ht="17" thickBot="1">
       <c r="A66" s="6"/>
       <c r="B66" s="15">
-        <f>B29+B6+B37+B43+B49+B58</f>
+        <f>B24+B6+B37+B43+B49+B58</f>
         <v>42</v>
       </c>
       <c r="J66" s="16">
-        <f>J35+J27+J41+J47+J56+J64</f>
-        <v>13</v>
+        <f>J35+J22+J41+J47+J56+J64</f>
+        <v>19</v>
       </c>
       <c r="K66" s="16">
-        <f>K35+K27+K41+K47+K56+K64</f>
+        <f>K35+K22+K41+K47+K56+K64</f>
         <v>1</v>
       </c>
       <c r="Q66" s="28"/>
@@ -5800,7 +5852,7 @@
     <row r="68" spans="1:20">
       <c r="A68" s="6"/>
       <c r="B68" s="17" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -5862,12 +5914,8 @@
       <c r="L70" s="8"/>
       <c r="M70" s="6"/>
       <c r="N70" s="8"/>
-      <c r="O70" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="P70" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O70" s="8"/>
+      <c r="P70" s="12"/>
       <c r="Q70" s="28"/>
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
@@ -5890,12 +5938,8 @@
       <c r="L71" s="8"/>
       <c r="M71" s="6"/>
       <c r="N71" s="8"/>
-      <c r="O71" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="P71" s="12" t="s">
-        <v>15</v>
-      </c>
+      <c r="O71" s="8"/>
+      <c r="P71" s="12"/>
       <c r="Q71" s="28"/>
       <c r="R71" s="9"/>
       <c r="S71" s="9"/>
@@ -5918,12 +5962,8 @@
       <c r="L72" s="8"/>
       <c r="M72" s="6"/>
       <c r="N72" s="8"/>
-      <c r="O72" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P72" s="12" t="s">
-        <v>17</v>
-      </c>
+      <c r="O72" s="8"/>
+      <c r="P72" s="12"/>
       <c r="Q72" s="28"/>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
@@ -6006,7 +6046,7 @@
         <v>45</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
@@ -6031,7 +6071,7 @@
         <v>5</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
@@ -6058,7 +6098,7 @@
         <v>50</v>
       </c>
       <c r="C78" s="25" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
@@ -11888,7 +11928,7 @@
   <mergeCells count="1">
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H27:H55 H68:H1048576 H1:H20">
+  <conditionalFormatting sqref="H1:H20 H68:H1048576 H22:H55">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -11900,27 +11940,27 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H59:H63">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+      <formula>"M"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
       <formula>"N"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
-      <formula>"M"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J27:J64 J66 J68:J248 J7:J20">
+  <conditionalFormatting sqref="J7:J20 J66 J68:J248 J22:J64">
     <cfRule type="notContainsBlanks" dxfId="2" priority="724">
       <formula>LEN(TRIM(J7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17">
+  <conditionalFormatting sqref="K17 K22:L38">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(K17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:L16 L18:L26 K27:L38 L39:L55 K40:K50 K56:K64 K62:L63 K66 K68:L248">
+  <conditionalFormatting sqref="K7:L16 L18:L21 L39:L55 K40:K50 K56:K64 K62:L63 K66 K68:L248">
     <cfRule type="notContainsBlanks" dxfId="0" priority="725">
       <formula>LEN(TRIM(K7))&gt;0</formula>
     </cfRule>
@@ -11935,12 +11975,12 @@
   <dimension ref="A1:BI246"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="139.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="83.5" customWidth="1"/>
     <col min="3" max="3" width="39.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12010,14 +12050,20 @@
     <row r="2" spans="1:61">
       <c r="A2" s="21"/>
       <c r="B2" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+        <v>15</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>34</v>
+      </c>
       <c r="G2" s="21"/>
       <c r="H2" s="21"/>
       <c r="I2" s="21"/>
@@ -12076,11 +12122,21 @@
     </row>
     <row r="3" spans="1:61">
       <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
+      <c r="B3" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="21">
+        <v>2024</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>100</v>
+      </c>
       <c r="G3" s="21"/>
       <c r="H3" s="21"/>
       <c r="I3" s="21"/>
@@ -12139,10 +12195,18 @@
     </row>
     <row r="4" spans="1:61">
       <c r="A4" s="21"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="21"/>
-      <c r="D4" s="21"/>
-      <c r="E4" s="21"/>
+      <c r="B4" s="21" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E4" s="21">
+        <v>2020</v>
+      </c>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="21"/>
@@ -12202,10 +12266,18 @@
     </row>
     <row r="5" spans="1:61">
       <c r="A5" s="21"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="B5" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" s="21">
+        <v>2023</v>
+      </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
       <c r="H5" s="21"/>

</xml_diff>

<commit_message>
update more detailed table of literature review
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F192A570-853F-664B-9F60-364C2155F495}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E5846B-BFD5-044A-83DE-4CDC161967A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="1" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
   <sheets>
     <sheet name="Four-phase flow diagram" sheetId="2" r:id="rId1"/>
     <sheet name="Analysis abstracts + criteria" sheetId="3" r:id="rId2"/>
     <sheet name="Untraceable articles" sheetId="4" r:id="rId3"/>
+    <sheet name="Overview" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="155">
   <si>
     <t>Google Scholar</t>
   </si>
@@ -566,12 +567,184 @@
   <si>
     <t>Massaoudi et al.</t>
   </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Decision/Actions</t>
+  </si>
+  <si>
+    <t>Pg, Vg</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Pd(t), Qd(t), Pg(t-1)</t>
+  </si>
+  <si>
+    <t>Pg(t), Vg(t)</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Methodolgy</t>
+  </si>
+  <si>
+    <t>Reward</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Clipped function with penalty</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+Line loading balance</t>
+  </si>
+  <si>
+    <t>DDPG  without critic network
+Lagrangian relaxation -&gt; to form objective function sbj. to constraints
+Interior point method -&gt; replace crictic network to determine the update direction of DNN parameter within feasibility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imitation Learning (IL) - initialization of policy (actor) NN for the DRL
+PPO
+</t>
+  </si>
+  <si>
+    <t>Problem Type</t>
+  </si>
+  <si>
+    <t>OPF</t>
+  </si>
+  <si>
+    <t>Wind generation availability
+Load balance
+Voltage violation
+Line loading balance
+BSS energy balance, storage capacity, PCS limitation</t>
+  </si>
+  <si>
+    <t>PPO+clipped function with penalty</t>
+  </si>
+  <si>
+    <t>wind generation
+BESS</t>
+  </si>
+  <si>
+    <t>Every different kind of power generation</t>
+  </si>
+  <si>
+    <t>Minimize generation cost + voltage fluctuation + power loss</t>
+  </si>
+  <si>
+    <t>Mulit-period OPF + BSS</t>
+  </si>
+  <si>
+    <t>Multi-objective OPF</t>
+  </si>
+  <si>
+    <t>P, Q, V, S</t>
+  </si>
+  <si>
+    <t>DDPG + MG-ASTGCN (multi-grained attention-based spatial-temporal graph convolution network)
+Weighting factor introduction for the multi-objective function</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation</t>
+  </si>
+  <si>
+    <t>TD3</t>
+  </si>
+  <si>
+    <t>Minimize generation cost</t>
+  </si>
+  <si>
+    <t>Minimize power loss</t>
+  </si>
+  <si>
+    <t>Pd, Qd, Pg, Vg</t>
+  </si>
+  <si>
+    <t>Pd, Qd, Pwind, SOC, ElecPrice</t>
+  </si>
+  <si>
+    <t>Pd, Qd</t>
+  </si>
+  <si>
+    <t>ΔPg, ΔVg</t>
+  </si>
+  <si>
+    <t>Pbss, Qbss, Qwind</t>
+  </si>
+  <si>
+    <t>Pc(controllable Pg), Vg</t>
+  </si>
+  <si>
+    <t>Pd, Qd, Pg, Vg, Ydiag</t>
+  </si>
+  <si>
+    <t>Remark</t>
+  </si>
+  <si>
+    <t>OPF + N-1 contigencies</t>
+  </si>
+  <si>
+    <t>SRL</t>
+  </si>
+  <si>
+    <t>Mulit-period OPF</t>
+  </si>
+  <si>
+    <t>Generation availability (ramping constraint included)
+Load balance
+Voltage violation
+Line loading balance</t>
+  </si>
+  <si>
+    <t>Pd(t) [net demand after subtracting renewable generation], Pg(t-1), Pg(t+1) [forecasted]</t>
+  </si>
+  <si>
+    <t>Convex constrained SAC (SAC + convexed safe layer)</t>
+  </si>
+  <si>
+    <t>PPO
+Initialization (behavior cloning) with OPF solver</t>
+  </si>
+  <si>
+    <t>X (safety layer)</t>
+  </si>
+  <si>
+    <t>X (Primal-dual)</t>
+  </si>
+  <si>
+    <t>Behavior cloning (BC)
+Architecture search druing BC
+PDO-based PPO
+Multi-processing training</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation (phase angle constraint included)
+Line loading balance</t>
+  </si>
+  <si>
+    <t>Clipped function with only divergence</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -622,6 +795,12 @@
       <i/>
       <sz val="8"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -831,7 +1010,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -899,47 +1078,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -956,6 +1097,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -971,16 +1115,66 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2356,23 +2550,23 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="29" t="s">
+      <c r="E2" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="30"/>
-      <c r="G2" s="31"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="43"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="33"/>
+      <c r="K2" s="50"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="29" t="s">
+      <c r="M2" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="30"/>
-      <c r="O2" s="31"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="33"/>
+      <c r="Q2" s="50"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2401,19 +2595,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="34"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="51"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="38"/>
+      <c r="K3" s="36"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="50"/>
+      <c r="O3" s="51"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="38"/>
+      <c r="Q3" s="36"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2442,19 +2636,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="37"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="46"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="38"/>
+      <c r="K4" s="36"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
+      <c r="M4" s="44"/>
+      <c r="N4" s="45"/>
+      <c r="O4" s="46"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="38"/>
+      <c r="Q4" s="36"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -2605,15 +2799,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="39" t="s">
+      <c r="D8" s="52" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="52" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="41" t="s">
+      <c r="H8" s="54" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -2652,11 +2846,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="40"/>
+      <c r="D9" s="53"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="40"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="42"/>
+      <c r="H9" s="55"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -2779,18 +2973,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="50"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="39"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="48" t="s">
+      <c r="M12" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="51"/>
-      <c r="O12" s="52"/>
+      <c r="N12" s="40"/>
+      <c r="O12" s="41"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -2906,18 +3100,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="50"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="48" t="s">
+      <c r="M15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="49"/>
-      <c r="O15" s="50"/>
+      <c r="N15" s="38"/>
+      <c r="O15" s="39"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -3033,18 +3227,18 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="29" t="s">
+      <c r="H18" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="30"/>
-      <c r="J18" s="31"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="43"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="29" t="s">
+      <c r="M18" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="44"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3078,14 +3272,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="35"/>
-      <c r="I19" s="36"/>
-      <c r="J19" s="37"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="45"/>
+      <c r="J19" s="46"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="45"/>
-      <c r="N19" s="46"/>
-      <c r="O19" s="47"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="35"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3201,11 +3395,11 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="29" t="s">
+      <c r="H22" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
+      <c r="I22" s="31"/>
+      <c r="J22" s="32"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3244,9 +3438,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="47"/>
+      <c r="H23" s="33"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="35"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3325,10 +3519,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="53" t="s">
+      <c r="G25" s="47" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="54"/>
+      <c r="H25" s="48"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
         <v>19</v>
@@ -3449,8 +3643,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="38"/>
-      <c r="E28" s="38"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -3980,6 +4174,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:G4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:O4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H22:J23"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="H12:J12"/>
@@ -3989,13 +4190,6 @@
     <mergeCell ref="H18:J19"/>
     <mergeCell ref="M18:O19"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="M2:O4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4007,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D301BBB3-8351-4307-9EEB-9EB9FA3A0E4E}">
   <dimension ref="A1:T346"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:F6"/>
+    <sheetView zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
@@ -4065,10 +4259,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="55" t="s">
+      <c r="J2" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="55"/>
+      <c r="K2" s="56"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>34</v>
@@ -4163,7 +4357,7 @@
     <row r="6" spans="1:20">
       <c r="A6" s="6"/>
       <c r="B6" s="12">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C6" s="13" t="s">
         <v>33</v>
@@ -4770,7 +4964,7 @@
     <row r="24" spans="1:20">
       <c r="A24" s="6"/>
       <c r="B24" s="12">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C24" s="13" t="s">
         <v>69</v>
@@ -5827,7 +6021,7 @@
       <c r="A66" s="6"/>
       <c r="B66" s="15">
         <f>B24+B6+B37+B43+B49+B58</f>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J66" s="16">
         <f>J35+J22+J41+J47+J56+J64</f>
@@ -6043,7 +6237,7 @@
       <c r="A76" s="6"/>
       <c r="B76" s="12">
         <f>B66+B74</f>
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C76" s="6" t="s">
         <v>21</v>
@@ -6095,7 +6289,7 @@
       <c r="A78" s="6"/>
       <c r="B78" s="24">
         <f>B77+B76</f>
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C78" s="25" t="s">
         <v>22</v>
@@ -11928,7 +12122,7 @@
   <mergeCells count="1">
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H20 H68:H1048576 H22:H55">
+  <conditionalFormatting sqref="H1:H20 H22:H55 H68:H1048576">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -11950,7 +12144,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J20 J66 J68:J248 J22:J64">
+  <conditionalFormatting sqref="J7:J20 J22:J64 J66 J68:J248">
     <cfRule type="notContainsBlanks" dxfId="2" priority="724">
       <formula>LEN(TRIM(J7))&gt;0</formula>
     </cfRule>
@@ -12061,7 +12255,7 @@
       <c r="E2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="56" t="s">
+      <c r="F2" s="29" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="21"/>
@@ -27522,4 +27716,369 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E329102-D1E6-314A-A75F-E468AE5BC4F5}">
+  <dimension ref="B2:N10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="7.83203125" customWidth="1"/>
+    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.33203125" customWidth="1"/>
+    <col min="12" max="12" width="56.5" customWidth="1"/>
+    <col min="13" max="13" width="14.5" customWidth="1"/>
+    <col min="14" max="14" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:14">
+      <c r="B2" s="57" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="57" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G2" s="57" t="s">
+        <v>106</v>
+      </c>
+      <c r="H2" s="57" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" s="57" t="s">
+        <v>109</v>
+      </c>
+      <c r="J2" s="57" t="s">
+        <v>114</v>
+      </c>
+      <c r="K2" s="57" t="s">
+        <v>112</v>
+      </c>
+      <c r="L2" s="57" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="57" t="s">
+        <v>144</v>
+      </c>
+      <c r="N2" s="57" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" ht="63" customHeight="1">
+      <c r="B3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="8">
+        <v>2020</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G3" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="58" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="K3" s="59" t="s">
+        <v>117</v>
+      </c>
+      <c r="L3" s="60" t="s">
+        <v>118</v>
+      </c>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="2:14" ht="64">
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="8">
+        <v>2020</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G4" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="H4" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="I4" s="58" t="s">
+        <v>135</v>
+      </c>
+      <c r="J4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="60" t="s">
+        <v>119</v>
+      </c>
+      <c r="M4" s="60"/>
+    </row>
+    <row r="5" spans="2:14" ht="96">
+      <c r="B5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2021</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" s="58" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="58" t="s">
+        <v>139</v>
+      </c>
+      <c r="I5" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="J5" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="60" t="s">
+        <v>122</v>
+      </c>
+      <c r="L5" s="58" t="s">
+        <v>123</v>
+      </c>
+      <c r="M5" s="58"/>
+      <c r="N5" s="59" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="64">
+      <c r="B6" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F6" s="61" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" s="58" t="s">
+        <v>126</v>
+      </c>
+      <c r="H6" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="I6" s="58" t="s">
+        <v>129</v>
+      </c>
+      <c r="J6" s="58" t="s">
+        <v>116</v>
+      </c>
+      <c r="K6" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="L6" s="60" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="60"/>
+      <c r="N6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" ht="48">
+      <c r="B7" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="62" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="63">
+        <v>2022</v>
+      </c>
+      <c r="F7" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="G7" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H7" s="58" t="s">
+        <v>140</v>
+      </c>
+      <c r="I7" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="J7" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="60" t="s">
+        <v>131</v>
+      </c>
+      <c r="L7" s="60" t="s">
+        <v>132</v>
+      </c>
+      <c r="M7" s="60"/>
+    </row>
+    <row r="8" spans="2:14" ht="64">
+      <c r="B8" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F8" s="61" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H8" s="58" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="58" t="s">
+        <v>141</v>
+      </c>
+      <c r="J8" t="s">
+        <v>116</v>
+      </c>
+      <c r="K8" s="60" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" s="60" t="s">
+        <v>149</v>
+      </c>
+      <c r="M8" s="60"/>
+    </row>
+    <row r="9" spans="2:14" ht="80">
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>145</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>147</v>
+      </c>
+      <c r="J9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K9" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="L9" s="60" t="s">
+        <v>148</v>
+      </c>
+      <c r="M9" s="60" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="80">
+      <c r="B10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F10" s="61" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="58" t="s">
+        <v>137</v>
+      </c>
+      <c r="J10" t="s">
+        <v>154</v>
+      </c>
+      <c r="K10" s="60" t="s">
+        <v>153</v>
+      </c>
+      <c r="L10" s="60" t="s">
+        <v>152</v>
+      </c>
+      <c r="M10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
reviewed on other math. opt. method for EV+OPF Problem
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E5846B-BFD5-044A-83DE-4CDC161967A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FAC372-3AF5-484F-92AB-677C94082D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="211">
   <si>
     <t>Google Scholar</t>
   </si>
@@ -623,13 +623,6 @@
     <t>OPF</t>
   </si>
   <si>
-    <t>Wind generation availability
-Load balance
-Voltage violation
-Line loading balance
-BSS energy balance, storage capacity, PCS limitation</t>
-  </si>
-  <si>
     <t>PPO+clipped function with penalty</t>
   </si>
   <si>
@@ -641,9 +634,6 @@
   </si>
   <si>
     <t>Minimize generation cost + voltage fluctuation + power loss</t>
-  </si>
-  <si>
-    <t>Mulit-period OPF + BSS</t>
   </si>
   <si>
     <t>Multi-objective OPF</t>
@@ -722,9 +712,6 @@
     <t>X (safety layer)</t>
   </si>
   <si>
-    <t>X (Primal-dual)</t>
-  </si>
-  <si>
     <t>Behavior cloning (BC)
 Architecture search druing BC
 PDO-based PPO
@@ -738,6 +725,228 @@
   </si>
   <si>
     <t>Clipped function with only divergence</t>
+  </si>
+  <si>
+    <t>Minimize generation cost + BESS power loss</t>
+  </si>
+  <si>
+    <t>Mulit-period OPF+BESS</t>
+  </si>
+  <si>
+    <t>Mulit-period OPF + BESS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pg, Qg, Pch/disch </t>
+  </si>
+  <si>
+    <t>V, SOC</t>
+  </si>
+  <si>
+    <t>- cost function</t>
+  </si>
+  <si>
+    <t>Wind generation availability
+Load balance
+Voltage violation
+Line loading balance
+BESS energy balance, storage capacity, PCS limitation</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+Line loading balance
+BESS charging rate limitation</t>
+  </si>
+  <si>
+    <t>X (Primal-dual Optimization)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TD3
+Primal-dual method: to enforce constraints
+Complex-valued Spatio-temporal graph Convolutional NN: to capture correlation of the environment states
+</t>
+  </si>
+  <si>
+    <t>Not OPF</t>
+  </si>
+  <si>
+    <t>"OPF" "EV"</t>
+  </si>
+  <si>
+    <t>The Promise of EV-Aware Multi-Period OPF Problem: Cost and Emission Benefits</t>
+  </si>
+  <si>
+    <t>Kayacık et al.</t>
+  </si>
+  <si>
+    <t>Sustainable Energy, Grids and Networks</t>
+  </si>
+  <si>
+    <t>Mulit-period OPF+EV</t>
+  </si>
+  <si>
+    <t>V, θ, Pch/disch, Pg, Qg, Pline, Qline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Second-Order Cone Programming (SOCP) relaxation
+</t>
+  </si>
+  <si>
+    <t>Symbiotic Organisms Search</t>
+  </si>
+  <si>
+    <t>Symbiotic organisms search algorithm-based security-constrained AC–DC OPF regarding uncertainty of wind, PV and PEV systems</t>
+  </si>
+  <si>
+    <t>Duman et al.</t>
+  </si>
+  <si>
+    <t>Soft Computing</t>
+  </si>
+  <si>
+    <t>AC-DC OPF+Contigency+EV</t>
+  </si>
+  <si>
+    <t>Pg, Vg, P(PV+EV), Qshunt, Ttrfo,the active and reactive power values of the rectifier and inverter sides, and id is the direct current</t>
+  </si>
+  <si>
+    <t>Minimize generation cost+emission cost+voltage deviation+line stress</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+Transformer, compensator limitation
+DC transmission link constraints</t>
+  </si>
+  <si>
+    <t>Scheduling of EV Battery Swapping—Part I: Centralized Solution</t>
+  </si>
+  <si>
+    <t>You et al.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEEE Transactions on Control of Network Systems </t>
+  </si>
+  <si>
+    <t>Optimal charging of electric vehicles in smart grid: Characterization and valley-filling algorithms</t>
+  </si>
+  <si>
+    <t>IEEE SmartGridComm 2012 Symposium - Architectures and Models</t>
+  </si>
+  <si>
+    <t>Minimize generation cost + EV charging cost</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+Line loading balance
+EV charging rate limitation
+EV charging demand
+Emission limitation</t>
+  </si>
+  <si>
+    <t>V^2, Pcharging</t>
+  </si>
+  <si>
+    <t>Valley-Filling Algorithm</t>
+  </si>
+  <si>
+    <t>A Stochastic Voltage Stability Constrained EMS for Isolated Microgrids in the Presence of PEVs Using a Coordinated UC-OPF Framework</t>
+  </si>
+  <si>
+    <t>Nikkhah et al.</t>
+  </si>
+  <si>
+    <t>IEEE Transactions on Industrial Electronics</t>
+  </si>
+  <si>
+    <t>Minimize generation cost+start-up+shut down</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+L-index
+Line loading balance
+EV charging rate limitation
+EV charging demand</t>
+  </si>
+  <si>
+    <t>Generation availability (including ramp-up/down)
+Load balance
+Voltage violation
+Line loading balance
+Spinning reserve requirements for generators
+L-index
+Wind &amp; PV generation
+BESS charging constraints
+EV charging capacity</t>
+  </si>
+  <si>
+    <t>OPF + Unit commitment(microgrid)</t>
+  </si>
+  <si>
+    <t>Mixed-integer non-linear programing (MINP)</t>
+  </si>
+  <si>
+    <t>Start-up, on/off, BESS dis/charging, EV dis/charging</t>
+  </si>
+  <si>
+    <t>Distribution Network Marginal Costs: Enhanced AC OPF Including Transformer Degradation</t>
+  </si>
+  <si>
+    <t>Andrianesis and Caramanis</t>
+  </si>
+  <si>
+    <t>Minimize generation cost+transformer degradation cost</t>
+  </si>
+  <si>
+    <t>Transformer-OPF</t>
+  </si>
+  <si>
+    <t>PchEV, PPV QchEV, QPV,
+trfo aging acceleration factor</t>
+  </si>
+  <si>
+    <t>OPF constraint
+DER constraint
+trfo constraint</t>
+  </si>
+  <si>
+    <t>DLMC framework</t>
+  </si>
+  <si>
+    <t>Multi-objective combined heat and power with wind–solar–EV of optimal power flow using hybrid evolutionary approach</t>
+  </si>
+  <si>
+    <t>Paul et al.</t>
+  </si>
+  <si>
+    <t>Electrical Engineering</t>
+  </si>
+  <si>
+    <t>Maximum utilization of renewable energy sources for economic power generation, minimize emission and reduced transmission losses</t>
+  </si>
+  <si>
+    <t>Metaheuristic: CDTBO (chaotic-opposition based driving training-based optimization)</t>
+  </si>
+  <si>
+    <t>Generation availability
+Load balance
+Voltage violation
+Line loading balance
+Transformer tap limitation
+EV (dis)charging rate limitation
+EV charging demand</t>
+  </si>
+  <si>
+    <t>Multi-objective  OPF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pg, Vg, Ttrfo, </t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1079,6 +1288,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1160,21 +1380,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2550,23 +2778,23 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="30" t="s">
+      <c r="E2" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="42"/>
-      <c r="G2" s="43"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="50"/>
+      <c r="K2" s="55"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="30" t="s">
+      <c r="M2" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="43"/>
+      <c r="N2" s="47"/>
+      <c r="O2" s="48"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="50"/>
+      <c r="Q2" s="55"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2595,19 +2823,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="51"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="56"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="36"/>
+      <c r="K3" s="41"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="49"/>
-      <c r="N3" s="50"/>
-      <c r="O3" s="51"/>
+      <c r="M3" s="54"/>
+      <c r="N3" s="55"/>
+      <c r="O3" s="56"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="36"/>
+      <c r="Q3" s="41"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2636,19 +2864,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="46"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="50"/>
+      <c r="G4" s="51"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="36"/>
+      <c r="K4" s="41"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="44"/>
-      <c r="N4" s="45"/>
-      <c r="O4" s="46"/>
+      <c r="M4" s="49"/>
+      <c r="N4" s="50"/>
+      <c r="O4" s="51"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="36"/>
+      <c r="Q4" s="41"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -2799,15 +3027,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="52" t="s">
+      <c r="D8" s="57" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="52" t="s">
+      <c r="F8" s="57" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="54" t="s">
+      <c r="H8" s="59" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -2846,11 +3074,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="53"/>
+      <c r="D9" s="58"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="53"/>
+      <c r="F9" s="58"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="55"/>
+      <c r="H9" s="60"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -2973,18 +3201,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="38"/>
-      <c r="J12" s="39"/>
+      <c r="I12" s="43"/>
+      <c r="J12" s="44"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="37" t="s">
+      <c r="M12" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="40"/>
-      <c r="O12" s="41"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="46"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -3100,18 +3328,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="38"/>
-      <c r="J15" s="39"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="44"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="37" t="s">
+      <c r="M15" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="38"/>
-      <c r="O15" s="39"/>
+      <c r="N15" s="43"/>
+      <c r="O15" s="44"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -3227,18 +3455,18 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="30" t="s">
+      <c r="H18" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="42"/>
-      <c r="J18" s="43"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="48"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="30" t="s">
+      <c r="M18" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="31"/>
-      <c r="O18" s="32"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="37"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3272,14 +3500,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="45"/>
-      <c r="J19" s="46"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="50"/>
+      <c r="J19" s="51"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="33"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="35"/>
+      <c r="M19" s="38"/>
+      <c r="N19" s="39"/>
+      <c r="O19" s="40"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3395,11 +3623,11 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="30" t="s">
+      <c r="H22" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="31"/>
-      <c r="J22" s="32"/>
+      <c r="I22" s="36"/>
+      <c r="J22" s="37"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3438,9 +3666,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="33"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="39"/>
+      <c r="J23" s="40"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3519,10 +3747,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="47" t="s">
+      <c r="G25" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="48"/>
+      <c r="H25" s="53"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
         <v>19</v>
@@ -3643,8 +3871,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -4199,17 +4427,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D301BBB3-8351-4307-9EEB-9EB9FA3A0E4E}">
-  <dimension ref="A1:T346"/>
+  <dimension ref="A1:T352"/>
   <sheetViews>
-    <sheetView zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14:F14"/>
+    <sheetView topLeftCell="A17" zoomScale="108" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.5" style="2" customWidth="1"/>
     <col min="2" max="2" width="4.5" style="2" customWidth="1"/>
-    <col min="3" max="3" width="87.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="59.5" style="2" customWidth="1"/>
     <col min="4" max="4" width="18.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="34.33203125" style="2" customWidth="1"/>
     <col min="6" max="6" width="6.5" style="2" customWidth="1"/>
@@ -4259,10 +4487,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="56"/>
+      <c r="K2" s="61"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>34</v>
@@ -4389,7 +4617,9 @@
       <c r="T6" s="9"/>
     </row>
     <row r="7" spans="1:20">
-      <c r="A7" s="6"/>
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B7" s="12">
         <v>1</v>
       </c>
@@ -4425,7 +4655,9 @@
       <c r="T7" s="9"/>
     </row>
     <row r="8" spans="1:20">
-      <c r="A8" s="6"/>
+      <c r="A8" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B8" s="12">
         <v>2</v>
       </c>
@@ -4461,7 +4693,9 @@
       <c r="T8" s="9"/>
     </row>
     <row r="9" spans="1:20">
-      <c r="A9" s="6"/>
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B9" s="12">
         <v>3</v>
       </c>
@@ -4497,7 +4731,9 @@
       <c r="T9" s="9"/>
     </row>
     <row r="10" spans="1:20">
-      <c r="A10" s="6"/>
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B10" s="12">
         <v>4</v>
       </c>
@@ -4533,7 +4769,9 @@
       <c r="T10" s="9"/>
     </row>
     <row r="11" spans="1:20">
-      <c r="A11" s="6"/>
+      <c r="A11" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B11" s="12">
         <v>5</v>
       </c>
@@ -4569,7 +4807,9 @@
       <c r="T11" s="9"/>
     </row>
     <row r="12" spans="1:20">
-      <c r="A12" s="6"/>
+      <c r="A12" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B12" s="12">
         <v>6</v>
       </c>
@@ -4605,7 +4845,9 @@
       <c r="T12" s="9"/>
     </row>
     <row r="13" spans="1:20">
-      <c r="A13" s="6"/>
+      <c r="A13" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B13" s="12">
         <v>7</v>
       </c>
@@ -4641,7 +4883,9 @@
       <c r="T13" s="9"/>
     </row>
     <row r="14" spans="1:20">
-      <c r="A14" s="6"/>
+      <c r="A14" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B14" s="12">
         <v>8</v>
       </c>
@@ -4677,7 +4921,9 @@
       <c r="T14" s="9"/>
     </row>
     <row r="15" spans="1:20">
-      <c r="A15" s="6"/>
+      <c r="A15" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="B15" s="12">
         <v>9</v>
       </c>
@@ -4847,7 +5093,9 @@
       </c>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
-      <c r="M19" s="6"/>
+      <c r="M19" s="6" t="s">
+        <v>162</v>
+      </c>
       <c r="N19" s="8"/>
       <c r="O19" s="8"/>
       <c r="P19" s="12"/>
@@ -5382,7 +5630,9 @@
     <row r="36" spans="1:20">
       <c r="A36" s="6"/>
       <c r="B36" s="12"/>
-      <c r="C36" s="6"/>
+      <c r="C36" s="14" t="s">
+        <v>163</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="8"/>
@@ -5404,16 +5654,28 @@
     <row r="37" spans="1:20">
       <c r="A37" s="6"/>
       <c r="B37" s="12">
-        <v>3</v>
-      </c>
-      <c r="C37" s="14"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="8"/>
+        <v>24</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="E37" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F37" s="8">
+        <v>2023</v>
+      </c>
       <c r="G37" s="8"/>
-      <c r="H37" s="8"/>
+      <c r="H37" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
+      <c r="J37" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K37" s="8"/>
       <c r="L37" s="8"/>
       <c r="M37" s="6"/>
@@ -5430,16 +5692,28 @@
     <row r="38" spans="1:20">
       <c r="A38" s="6"/>
       <c r="B38" s="12">
-        <v>26</v>
-      </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="8"/>
+        <v>25</v>
+      </c>
+      <c r="C38" t="s">
+        <v>171</v>
+      </c>
+      <c r="D38" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="E38" t="s">
+        <v>173</v>
+      </c>
+      <c r="F38" s="62">
+        <v>2021</v>
+      </c>
       <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="H38" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
+      <c r="J38" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="6"/>
@@ -5454,16 +5728,29 @@
     <row r="39" spans="1:20">
       <c r="A39" s="6"/>
       <c r="B39" s="12">
-        <v>27</v>
-      </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="8"/>
+        <v>26</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F39" s="8">
+        <v>2017</v>
+      </c>
       <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+      <c r="H39" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I39" s="8"/>
       <c r="J39" s="8"/>
+      <c r="K39" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="L39" s="8"/>
       <c r="M39" s="6"/>
       <c r="N39" s="8"/>
@@ -5477,16 +5764,28 @@
     <row r="40" spans="1:20">
       <c r="A40" s="6"/>
       <c r="B40" s="12">
-        <v>28</v>
-      </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="8"/>
+        <v>27</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F40" s="8">
+        <v>2012</v>
+      </c>
       <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="H40" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
+      <c r="J40" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="6"/>
@@ -5500,20 +5799,30 @@
     </row>
     <row r="41" spans="1:20">
       <c r="A41" s="6"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="8"/>
+      <c r="B41" s="12">
+        <v>28</v>
+      </c>
+      <c r="C41" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="D41" t="s">
+        <v>188</v>
+      </c>
+      <c r="E41" t="s">
+        <v>189</v>
+      </c>
+      <c r="F41" s="62">
+        <v>2021</v>
+      </c>
       <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="H41" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I41" s="8"/>
-      <c r="J41" s="8">
-        <v>0</v>
-      </c>
-      <c r="K41" s="8">
-        <v>0</v>
-      </c>
+      <c r="J41" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="K41" s="8"/>
       <c r="L41" s="8"/>
       <c r="M41" s="6"/>
       <c r="N41" s="8"/>
@@ -5526,15 +5835,29 @@
     </row>
     <row r="42" spans="1:20">
       <c r="A42" s="6"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-      <c r="F42" s="8"/>
+      <c r="B42" s="12">
+        <v>29</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="F42" s="8">
+        <v>2020</v>
+      </c>
       <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="H42" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
+      <c r="J42" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
       <c r="M42" s="6"/>
@@ -5549,16 +5872,28 @@
     <row r="43" spans="1:20">
       <c r="A43" s="6"/>
       <c r="B43" s="12">
-        <v>3</v>
-      </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="C43" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="D43" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="E43" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" s="62">
+        <v>2024</v>
+      </c>
       <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
+      <c r="H43" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
+      <c r="J43" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="K43" s="8"/>
       <c r="L43" s="8"/>
       <c r="M43" s="6"/>
@@ -5566,16 +5901,14 @@
       <c r="O43" s="8"/>
       <c r="P43" s="12"/>
       <c r="Q43" s="28"/>
-      <c r="R43" s="9">
-        <v>158</v>
-      </c>
+      <c r="R43" s="9"/>
       <c r="S43" s="9"/>
       <c r="T43" s="9"/>
     </row>
     <row r="44" spans="1:20">
       <c r="A44" s="6"/>
       <c r="B44" s="12">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
@@ -5599,7 +5932,7 @@
     <row r="45" spans="1:20">
       <c r="A45" s="6"/>
       <c r="B45" s="12">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
@@ -5609,7 +5942,6 @@
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
       <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
       <c r="L45" s="8"/>
       <c r="M45" s="6"/>
       <c r="N45" s="8"/>
@@ -5623,7 +5955,7 @@
     <row r="46" spans="1:20">
       <c r="A46" s="6"/>
       <c r="B46" s="12">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
@@ -5661,6 +5993,7 @@
         <v>0</v>
       </c>
       <c r="L47" s="8"/>
+      <c r="M47" s="6"/>
       <c r="N47" s="8"/>
       <c r="O47" s="8"/>
       <c r="P47" s="12"/>
@@ -5694,9 +6027,9 @@
     <row r="49" spans="1:20">
       <c r="A49" s="6"/>
       <c r="B49" s="12">
-        <v>6</v>
-      </c>
-      <c r="C49" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="C49" s="13"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="8"/>
@@ -5712,7 +6045,7 @@
       <c r="P49" s="12"/>
       <c r="Q49" s="28"/>
       <c r="R49" s="9">
-        <v>438</v>
+        <v>158</v>
       </c>
       <c r="S49" s="9"/>
       <c r="T49" s="9"/>
@@ -5720,7 +6053,7 @@
     <row r="50" spans="1:20">
       <c r="A50" s="6"/>
       <c r="B50" s="12">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C50" s="6"/>
       <c r="D50" s="6"/>
@@ -5744,7 +6077,7 @@
     <row r="51" spans="1:20">
       <c r="A51" s="6"/>
       <c r="B51" s="12">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -5754,6 +6087,7 @@
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
       <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
       <c r="L51" s="8"/>
       <c r="M51" s="6"/>
       <c r="N51" s="8"/>
@@ -5767,7 +6101,7 @@
     <row r="52" spans="1:20">
       <c r="A52" s="6"/>
       <c r="B52" s="12">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -5777,6 +6111,7 @@
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
       <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
       <c r="L52" s="8"/>
       <c r="M52" s="6"/>
       <c r="N52" s="8"/>
@@ -5789,9 +6124,7 @@
     </row>
     <row r="53" spans="1:20">
       <c r="A53" s="6"/>
-      <c r="B53" s="12">
-        <v>35</v>
-      </c>
+      <c r="B53" s="12"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
       <c r="E53" s="6"/>
@@ -5799,9 +6132,13 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
+      <c r="J53" s="8">
+        <v>0</v>
+      </c>
+      <c r="K53" s="8">
+        <v>0</v>
+      </c>
       <c r="L53" s="8"/>
-      <c r="M53" s="6"/>
       <c r="N53" s="8"/>
       <c r="O53" s="8"/>
       <c r="P53" s="12"/>
@@ -5812,9 +6149,7 @@
     </row>
     <row r="54" spans="1:20">
       <c r="A54" s="6"/>
-      <c r="B54" s="12">
-        <v>36</v>
-      </c>
+      <c r="B54" s="12"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
       <c r="E54" s="6"/>
@@ -5823,6 +6158,7 @@
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
       <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
       <c r="L54" s="8"/>
       <c r="M54" s="6"/>
       <c r="N54" s="8"/>
@@ -5836,9 +6172,9 @@
     <row r="55" spans="1:20">
       <c r="A55" s="6"/>
       <c r="B55" s="12">
-        <v>37</v>
-      </c>
-      <c r="C55" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C55" s="14"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
       <c r="F55" s="8"/>
@@ -5846,24 +6182,38 @@
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
       <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
       <c r="L55" s="8"/>
       <c r="M55" s="6"/>
       <c r="N55" s="8"/>
       <c r="O55" s="8"/>
       <c r="P55" s="12"/>
       <c r="Q55" s="28"/>
-      <c r="R55" s="9"/>
+      <c r="R55" s="9">
+        <v>438</v>
+      </c>
       <c r="S55" s="9"/>
       <c r="T55" s="9"/>
     </row>
     <row r="56" spans="1:20">
       <c r="A56" s="6"/>
-      <c r="J56" s="8">
-        <v>0</v>
-      </c>
-      <c r="K56" s="8">
-        <v>0</v>
-      </c>
+      <c r="B56" s="12">
+        <v>32</v>
+      </c>
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="8"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+      <c r="L56" s="8"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="8"/>
+      <c r="O56" s="8"/>
+      <c r="P56" s="12"/>
       <c r="Q56" s="28"/>
       <c r="R56" s="9"/>
       <c r="S56" s="9"/>
@@ -5871,8 +6221,22 @@
     </row>
     <row r="57" spans="1:20">
       <c r="A57" s="6"/>
+      <c r="B57" s="12">
+        <v>33</v>
+      </c>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="8"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
       <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
+      <c r="L57" s="8"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="8"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="12"/>
       <c r="Q57" s="28"/>
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
@@ -5881,48 +6245,65 @@
     <row r="58" spans="1:20">
       <c r="A58" s="6"/>
       <c r="B58" s="12">
-        <v>5</v>
-      </c>
-      <c r="C58" s="14"/>
+        <v>34</v>
+      </c>
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="8"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
       <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
+      <c r="L58" s="8"/>
+      <c r="M58" s="6"/>
+      <c r="N58" s="8"/>
+      <c r="O58" s="8"/>
+      <c r="P58" s="12"/>
       <c r="Q58" s="28"/>
-      <c r="R58" s="9">
-        <v>649</v>
-      </c>
+      <c r="R58" s="9"/>
       <c r="S58" s="9"/>
       <c r="T58" s="9"/>
     </row>
     <row r="59" spans="1:20">
       <c r="A59" s="6"/>
       <c r="B59" s="12">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
       <c r="F59" s="8"/>
+      <c r="G59" s="8"/>
       <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
       <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
+      <c r="L59" s="8"/>
+      <c r="M59" s="6"/>
+      <c r="N59" s="8"/>
       <c r="O59" s="8"/>
       <c r="P59" s="12"/>
       <c r="Q59" s="28"/>
+      <c r="R59" s="9"/>
       <c r="S59" s="9"/>
       <c r="T59" s="9"/>
     </row>
     <row r="60" spans="1:20">
       <c r="A60" s="6"/>
       <c r="B60" s="12">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
       <c r="E60" s="6"/>
       <c r="F60" s="8"/>
+      <c r="G60" s="8"/>
       <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
       <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
+      <c r="L60" s="8"/>
+      <c r="M60" s="6"/>
+      <c r="N60" s="8"/>
       <c r="O60" s="8"/>
       <c r="P60" s="12"/>
       <c r="Q60" s="28"/>
@@ -5933,15 +6314,19 @@
     <row r="61" spans="1:20">
       <c r="A61" s="6"/>
       <c r="B61" s="12">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
       <c r="E61" s="6"/>
       <c r="F61" s="8"/>
+      <c r="G61" s="8"/>
       <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
       <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
+      <c r="L61" s="8"/>
+      <c r="M61" s="6"/>
+      <c r="N61" s="8"/>
       <c r="O61" s="8"/>
       <c r="P61" s="12"/>
       <c r="Q61" s="28"/>
@@ -5951,23 +6336,12 @@
     </row>
     <row r="62" spans="1:20">
       <c r="A62" s="6"/>
-      <c r="B62" s="12">
-        <v>41</v>
-      </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="6"/>
-      <c r="E62" s="6"/>
-      <c r="F62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="8"/>
-      <c r="M62" s="6"/>
-      <c r="N62" s="8"/>
-      <c r="O62" s="8"/>
-      <c r="P62" s="12"/>
+      <c r="J62" s="8">
+        <v>0</v>
+      </c>
+      <c r="K62" s="8">
+        <v>0</v>
+      </c>
       <c r="Q62" s="28"/>
       <c r="R62" s="9"/>
       <c r="S62" s="9"/>
@@ -5975,23 +6349,8 @@
     </row>
     <row r="63" spans="1:20">
       <c r="A63" s="6"/>
-      <c r="B63" s="12">
-        <v>42</v>
-      </c>
-      <c r="C63" s="6"/>
-      <c r="D63" s="6"/>
-      <c r="E63" s="6"/>
-      <c r="F63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
-      <c r="L63" s="8"/>
-      <c r="M63" s="6"/>
-      <c r="N63" s="8"/>
-      <c r="O63" s="8"/>
-      <c r="P63" s="12"/>
       <c r="Q63" s="28"/>
       <c r="R63" s="9"/>
       <c r="S63" s="9"/>
@@ -5999,45 +6358,70 @@
     </row>
     <row r="64" spans="1:20">
       <c r="A64" s="6"/>
-      <c r="J64" s="8">
-        <v>0</v>
-      </c>
-      <c r="K64" s="8">
-        <v>0</v>
-      </c>
+      <c r="B64" s="12">
+        <v>5</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
       <c r="Q64" s="28"/>
-      <c r="R64" s="9"/>
+      <c r="R64" s="9">
+        <v>649</v>
+      </c>
       <c r="S64" s="9"/>
       <c r="T64" s="9"/>
     </row>
     <row r="65" spans="1:20">
       <c r="A65" s="6"/>
+      <c r="B65" s="12">
+        <v>38</v>
+      </c>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="12"/>
       <c r="Q65" s="28"/>
-      <c r="R65" s="9"/>
       <c r="S65" s="9"/>
       <c r="T65" s="9"/>
     </row>
-    <row r="66" spans="1:20" ht="17" thickBot="1">
+    <row r="66" spans="1:20">
       <c r="A66" s="6"/>
-      <c r="B66" s="15">
-        <f>B24+B6+B37+B43+B49+B58</f>
-        <v>40</v>
-      </c>
-      <c r="J66" s="16">
-        <f>J35+J22+J41+J47+J56+J64</f>
-        <v>19</v>
-      </c>
-      <c r="K66" s="16">
-        <f>K35+K22+K41+K47+K56+K64</f>
-        <v>1</v>
-      </c>
+      <c r="B66" s="12">
+        <v>39</v>
+      </c>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+      <c r="O66" s="8"/>
+      <c r="P66" s="12"/>
       <c r="Q66" s="28"/>
       <c r="R66" s="9"/>
       <c r="S66" s="9"/>
       <c r="T66" s="9"/>
     </row>
-    <row r="67" spans="1:20" ht="17" thickTop="1">
+    <row r="67" spans="1:20">
       <c r="A67" s="6"/>
+      <c r="B67" s="12">
+        <v>40</v>
+      </c>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+      <c r="O67" s="8"/>
+      <c r="P67" s="12"/>
       <c r="Q67" s="28"/>
       <c r="R67" s="9"/>
       <c r="S67" s="9"/>
@@ -6045,8 +6429,8 @@
     </row>
     <row r="68" spans="1:20">
       <c r="A68" s="6"/>
-      <c r="B68" s="17" t="s">
-        <v>14</v>
+      <c r="B68" s="12">
+        <v>41</v>
       </c>
       <c r="C68" s="6"/>
       <c r="D68" s="6"/>
@@ -6063,15 +6447,15 @@
       <c r="O68" s="8"/>
       <c r="P68" s="12"/>
       <c r="Q68" s="28"/>
-      <c r="R68" s="9">
-        <v>3</v>
-      </c>
+      <c r="R68" s="9"/>
       <c r="S68" s="9"/>
       <c r="T68" s="9"/>
     </row>
     <row r="69" spans="1:20">
       <c r="A69" s="6"/>
-      <c r="B69" s="12"/>
+      <c r="B69" s="12">
+        <v>42</v>
+      </c>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
       <c r="E69" s="6"/>
@@ -6093,23 +6477,12 @@
     </row>
     <row r="70" spans="1:20">
       <c r="A70" s="6"/>
-      <c r="B70" s="12">
-        <v>43</v>
-      </c>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="F70" s="8"/>
-      <c r="G70" s="8"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="8"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="8"/>
-      <c r="O70" s="8"/>
-      <c r="P70" s="12"/>
+      <c r="J70" s="8">
+        <v>0</v>
+      </c>
+      <c r="K70" s="8">
+        <v>0</v>
+      </c>
       <c r="Q70" s="28"/>
       <c r="R70" s="9"/>
       <c r="S70" s="9"/>
@@ -6117,81 +6490,41 @@
     </row>
     <row r="71" spans="1:20">
       <c r="A71" s="6"/>
-      <c r="B71" s="12">
-        <v>44</v>
-      </c>
-      <c r="C71" s="6"/>
-      <c r="D71" s="6"/>
-      <c r="E71" s="6"/>
-      <c r="F71" s="8"/>
-      <c r="G71" s="8"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="8"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="8"/>
-      <c r="O71" s="8"/>
-      <c r="P71" s="12"/>
       <c r="Q71" s="28"/>
       <c r="R71" s="9"/>
       <c r="S71" s="9"/>
       <c r="T71" s="9"/>
     </row>
-    <row r="72" spans="1:20">
+    <row r="72" spans="1:20" ht="17" thickBot="1">
       <c r="A72" s="6"/>
-      <c r="B72" s="12">
-        <v>45</v>
-      </c>
-      <c r="C72" s="6"/>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6"/>
-      <c r="F72" s="8"/>
-      <c r="G72" s="8"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="8"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="8"/>
-      <c r="O72" s="8"/>
-      <c r="P72" s="12"/>
+      <c r="B72" s="15">
+        <f>B24+B6+B37+B49+B55+B64</f>
+        <v>61</v>
+      </c>
+      <c r="J72" s="16">
+        <f>J35+J22+J47+J53+J62+J70</f>
+        <v>19</v>
+      </c>
+      <c r="K72" s="16">
+        <f>K35+K22+K47+K53+K62+K70</f>
+        <v>1</v>
+      </c>
       <c r="Q72" s="28"/>
       <c r="R72" s="9"/>
       <c r="S72" s="9"/>
       <c r="T72" s="9"/>
     </row>
-    <row r="73" spans="1:20">
+    <row r="73" spans="1:20" ht="17" thickTop="1">
       <c r="A73" s="6"/>
-      <c r="C73" s="6"/>
-      <c r="D73" s="6"/>
-      <c r="E73" s="6"/>
-      <c r="F73" s="8"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8">
-        <v>0</v>
-      </c>
-      <c r="K73" s="8">
-        <v>0</v>
-      </c>
-      <c r="L73" s="8"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="8"/>
-      <c r="O73" s="8"/>
-      <c r="P73" s="12"/>
-      <c r="Q73" s="9"/>
+      <c r="Q73" s="28"/>
       <c r="R73" s="9"/>
       <c r="S73" s="9"/>
       <c r="T73" s="9"/>
     </row>
-    <row r="74" spans="1:20" ht="17" thickBot="1">
+    <row r="74" spans="1:20">
       <c r="A74" s="6"/>
-      <c r="B74" s="15">
-        <v>3</v>
+      <c r="B74" s="17" t="s">
+        <v>14</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
@@ -6207,12 +6540,14 @@
       <c r="N74" s="8"/>
       <c r="O74" s="8"/>
       <c r="P74" s="12"/>
-      <c r="Q74" s="9"/>
-      <c r="R74" s="9"/>
+      <c r="Q74" s="28"/>
+      <c r="R74" s="9">
+        <v>3</v>
+      </c>
       <c r="S74" s="9"/>
       <c r="T74" s="9"/>
     </row>
-    <row r="75" spans="1:20" ht="17" thickTop="1">
+    <row r="75" spans="1:20">
       <c r="A75" s="6"/>
       <c r="B75" s="12"/>
       <c r="C75" s="6"/>
@@ -6220,6 +6555,7 @@
       <c r="E75" s="6"/>
       <c r="F75" s="8"/>
       <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
       <c r="I75" s="8"/>
       <c r="J75" s="8"/>
       <c r="K75" s="8"/>
@@ -6228,7 +6564,7 @@
       <c r="N75" s="8"/>
       <c r="O75" s="8"/>
       <c r="P75" s="12"/>
-      <c r="Q75" s="9"/>
+      <c r="Q75" s="28"/>
       <c r="R75" s="9"/>
       <c r="S75" s="9"/>
       <c r="T75" s="9"/>
@@ -6236,16 +6572,14 @@
     <row r="76" spans="1:20">
       <c r="A76" s="6"/>
       <c r="B76" s="12">
-        <f>B66+B74</f>
         <v>43</v>
       </c>
-      <c r="C76" s="6" t="s">
-        <v>21</v>
-      </c>
+      <c r="C76" s="6"/>
       <c r="D76" s="6"/>
       <c r="E76" s="6"/>
       <c r="F76" s="8"/>
       <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
       <c r="I76" s="8"/>
       <c r="J76" s="8"/>
       <c r="K76" s="8"/>
@@ -6254,7 +6588,7 @@
       <c r="N76" s="8"/>
       <c r="O76" s="8"/>
       <c r="P76" s="12"/>
-      <c r="Q76" s="9"/>
+      <c r="Q76" s="28"/>
       <c r="R76" s="9"/>
       <c r="S76" s="9"/>
       <c r="T76" s="9"/>
@@ -6262,11 +6596,9 @@
     <row r="77" spans="1:20">
       <c r="A77" s="6"/>
       <c r="B77" s="12">
-        <v>5</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>20</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C77" s="6"/>
       <c r="D77" s="6"/>
       <c r="E77" s="6"/>
       <c r="F77" s="8"/>
@@ -6280,20 +6612,17 @@
       <c r="N77" s="8"/>
       <c r="O77" s="8"/>
       <c r="P77" s="12"/>
-      <c r="Q77" s="9"/>
+      <c r="Q77" s="28"/>
       <c r="R77" s="9"/>
       <c r="S77" s="9"/>
       <c r="T77" s="9"/>
     </row>
-    <row r="78" spans="1:20" ht="17" thickBot="1">
+    <row r="78" spans="1:20">
       <c r="A78" s="6"/>
-      <c r="B78" s="24">
-        <f>B77+B76</f>
-        <v>48</v>
-      </c>
-      <c r="C78" s="25" t="s">
-        <v>22</v>
-      </c>
+      <c r="B78" s="12">
+        <v>45</v>
+      </c>
+      <c r="C78" s="6"/>
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="8"/>
@@ -6307,14 +6636,13 @@
       <c r="N78" s="8"/>
       <c r="O78" s="8"/>
       <c r="P78" s="12"/>
-      <c r="Q78" s="9"/>
+      <c r="Q78" s="28"/>
       <c r="R78" s="9"/>
       <c r="S78" s="9"/>
       <c r="T78" s="9"/>
     </row>
-    <row r="79" spans="1:20" ht="17" thickTop="1">
+    <row r="79" spans="1:20">
       <c r="A79" s="6"/>
-      <c r="B79" s="12"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
       <c r="E79" s="6"/>
@@ -6322,8 +6650,12 @@
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
+      <c r="J79" s="8">
+        <v>0</v>
+      </c>
+      <c r="K79" s="8">
+        <v>0</v>
+      </c>
       <c r="L79" s="8"/>
       <c r="M79" s="6"/>
       <c r="N79" s="8"/>
@@ -6334,9 +6666,11 @@
       <c r="S79" s="9"/>
       <c r="T79" s="9"/>
     </row>
-    <row r="80" spans="1:20">
+    <row r="80" spans="1:20" ht="17" thickBot="1">
       <c r="A80" s="6"/>
-      <c r="B80" s="12"/>
+      <c r="B80" s="15">
+        <v>3</v>
+      </c>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
       <c r="E80" s="6"/>
@@ -6356,7 +6690,7 @@
       <c r="S80" s="9"/>
       <c r="T80" s="9"/>
     </row>
-    <row r="81" spans="1:20">
+    <row r="81" spans="1:20" ht="17" thickTop="1">
       <c r="A81" s="6"/>
       <c r="B81" s="12"/>
       <c r="C81" s="6"/>
@@ -6364,7 +6698,6 @@
       <c r="E81" s="6"/>
       <c r="F81" s="8"/>
       <c r="G81" s="8"/>
-      <c r="H81" s="8"/>
       <c r="I81" s="8"/>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
@@ -6380,20 +6713,24 @@
     </row>
     <row r="82" spans="1:20">
       <c r="A82" s="6"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="6"/>
+      <c r="B82" s="12">
+        <f>B72+B80</f>
+        <v>64</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>21</v>
+      </c>
       <c r="D82" s="6"/>
       <c r="E82" s="6"/>
       <c r="F82" s="8"/>
       <c r="G82" s="8"/>
-      <c r="H82" s="8"/>
       <c r="I82" s="8"/>
       <c r="J82" s="8"/>
       <c r="K82" s="8"/>
       <c r="L82" s="8"/>
       <c r="M82" s="6"/>
       <c r="N82" s="8"/>
-      <c r="O82" s="6"/>
+      <c r="O82" s="8"/>
       <c r="P82" s="12"/>
       <c r="Q82" s="9"/>
       <c r="R82" s="9"/>
@@ -6402,8 +6739,12 @@
     </row>
     <row r="83" spans="1:20">
       <c r="A83" s="6"/>
-      <c r="B83" s="12"/>
-      <c r="C83" s="6"/>
+      <c r="B83" s="12">
+        <v>5</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="D83" s="6"/>
       <c r="E83" s="6"/>
       <c r="F83" s="8"/>
@@ -6415,17 +6756,22 @@
       <c r="L83" s="8"/>
       <c r="M83" s="6"/>
       <c r="N83" s="8"/>
-      <c r="O83" s="6"/>
+      <c r="O83" s="8"/>
       <c r="P83" s="12"/>
       <c r="Q83" s="9"/>
       <c r="R83" s="9"/>
       <c r="S83" s="9"/>
       <c r="T83" s="9"/>
     </row>
-    <row r="84" spans="1:20">
+    <row r="84" spans="1:20" ht="17" thickBot="1">
       <c r="A84" s="6"/>
-      <c r="B84" s="12"/>
-      <c r="C84" s="6"/>
+      <c r="B84" s="24">
+        <f>B83+B82</f>
+        <v>69</v>
+      </c>
+      <c r="C84" s="25" t="s">
+        <v>22</v>
+      </c>
       <c r="D84" s="6"/>
       <c r="E84" s="6"/>
       <c r="F84" s="8"/>
@@ -6437,14 +6783,14 @@
       <c r="L84" s="8"/>
       <c r="M84" s="6"/>
       <c r="N84" s="8"/>
-      <c r="O84" s="6"/>
+      <c r="O84" s="8"/>
       <c r="P84" s="12"/>
       <c r="Q84" s="9"/>
       <c r="R84" s="9"/>
       <c r="S84" s="9"/>
       <c r="T84" s="9"/>
     </row>
-    <row r="85" spans="1:20">
+    <row r="85" spans="1:20" ht="17" thickTop="1">
       <c r="A85" s="6"/>
       <c r="B85" s="12"/>
       <c r="C85" s="6"/>
@@ -6459,7 +6805,7 @@
       <c r="L85" s="8"/>
       <c r="M85" s="6"/>
       <c r="N85" s="8"/>
-      <c r="O85" s="6"/>
+      <c r="O85" s="8"/>
       <c r="P85" s="12"/>
       <c r="Q85" s="9"/>
       <c r="R85" s="9"/>
@@ -6481,7 +6827,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="6"/>
       <c r="N86" s="8"/>
-      <c r="O86" s="6"/>
+      <c r="O86" s="8"/>
       <c r="P86" s="12"/>
       <c r="Q86" s="9"/>
       <c r="R86" s="9"/>
@@ -6503,7 +6849,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="6"/>
       <c r="N87" s="8"/>
-      <c r="O87" s="6"/>
+      <c r="O87" s="8"/>
       <c r="P87" s="12"/>
       <c r="Q87" s="9"/>
       <c r="R87" s="9"/>
@@ -8800,7 +9146,7 @@
     </row>
     <row r="192" spans="1:20">
       <c r="A192" s="6"/>
-      <c r="B192" s="6"/>
+      <c r="B192" s="12"/>
       <c r="C192" s="6"/>
       <c r="D192" s="6"/>
       <c r="E192" s="6"/>
@@ -8822,7 +9168,7 @@
     </row>
     <row r="193" spans="1:20">
       <c r="A193" s="6"/>
-      <c r="B193" s="6"/>
+      <c r="B193" s="12"/>
       <c r="C193" s="6"/>
       <c r="D193" s="6"/>
       <c r="E193" s="6"/>
@@ -8844,7 +9190,7 @@
     </row>
     <row r="194" spans="1:20">
       <c r="A194" s="6"/>
-      <c r="B194" s="6"/>
+      <c r="B194" s="12"/>
       <c r="C194" s="6"/>
       <c r="D194" s="6"/>
       <c r="E194" s="6"/>
@@ -8866,7 +9212,7 @@
     </row>
     <row r="195" spans="1:20">
       <c r="A195" s="6"/>
-      <c r="B195" s="6"/>
+      <c r="B195" s="12"/>
       <c r="C195" s="6"/>
       <c r="D195" s="6"/>
       <c r="E195" s="6"/>
@@ -8888,7 +9234,7 @@
     </row>
     <row r="196" spans="1:20">
       <c r="A196" s="6"/>
-      <c r="B196" s="6"/>
+      <c r="B196" s="12"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6"/>
       <c r="E196" s="6"/>
@@ -8910,7 +9256,7 @@
     </row>
     <row r="197" spans="1:20">
       <c r="A197" s="6"/>
-      <c r="B197" s="6"/>
+      <c r="B197" s="12"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6"/>
       <c r="E197" s="6"/>
@@ -9364,7 +9710,7 @@
       <c r="M217" s="6"/>
       <c r="N217" s="8"/>
       <c r="O217" s="6"/>
-      <c r="P217" s="6"/>
+      <c r="P217" s="12"/>
       <c r="Q217" s="9"/>
       <c r="R217" s="9"/>
       <c r="S217" s="9"/>
@@ -9386,7 +9732,7 @@
       <c r="M218" s="6"/>
       <c r="N218" s="8"/>
       <c r="O218" s="6"/>
-      <c r="P218" s="6"/>
+      <c r="P218" s="12"/>
       <c r="Q218" s="9"/>
       <c r="R218" s="9"/>
       <c r="S218" s="9"/>
@@ -9408,7 +9754,7 @@
       <c r="M219" s="6"/>
       <c r="N219" s="8"/>
       <c r="O219" s="6"/>
-      <c r="P219" s="6"/>
+      <c r="P219" s="12"/>
       <c r="Q219" s="9"/>
       <c r="R219" s="9"/>
       <c r="S219" s="9"/>
@@ -9430,7 +9776,7 @@
       <c r="M220" s="6"/>
       <c r="N220" s="8"/>
       <c r="O220" s="6"/>
-      <c r="P220" s="6"/>
+      <c r="P220" s="12"/>
       <c r="Q220" s="9"/>
       <c r="R220" s="9"/>
       <c r="S220" s="9"/>
@@ -9452,7 +9798,7 @@
       <c r="M221" s="6"/>
       <c r="N221" s="8"/>
       <c r="O221" s="6"/>
-      <c r="P221" s="6"/>
+      <c r="P221" s="12"/>
       <c r="Q221" s="9"/>
       <c r="R221" s="9"/>
       <c r="S221" s="9"/>
@@ -9474,7 +9820,7 @@
       <c r="M222" s="6"/>
       <c r="N222" s="8"/>
       <c r="O222" s="6"/>
-      <c r="P222" s="6"/>
+      <c r="P222" s="12"/>
       <c r="Q222" s="9"/>
       <c r="R222" s="9"/>
       <c r="S222" s="9"/>
@@ -10252,7 +10598,7 @@
     </row>
     <row r="258" spans="1:20">
       <c r="A258" s="6"/>
-      <c r="B258" s="9"/>
+      <c r="B258" s="6"/>
       <c r="C258" s="6"/>
       <c r="D258" s="6"/>
       <c r="E258" s="6"/>
@@ -10274,8 +10620,8 @@
     </row>
     <row r="259" spans="1:20">
       <c r="A259" s="6"/>
-      <c r="B259" s="9"/>
-      <c r="C259" s="9"/>
+      <c r="B259" s="6"/>
+      <c r="C259" s="6"/>
       <c r="D259" s="6"/>
       <c r="E259" s="6"/>
       <c r="F259" s="8"/>
@@ -10295,126 +10641,132 @@
       <c r="T259" s="9"/>
     </row>
     <row r="260" spans="1:20">
-      <c r="B260" s="9"/>
-      <c r="C260" s="9"/>
-      <c r="D260" s="9"/>
-      <c r="E260" s="9"/>
-      <c r="F260" s="18"/>
-      <c r="G260" s="18"/>
-      <c r="H260" s="18"/>
-      <c r="I260" s="18"/>
-      <c r="J260" s="18"/>
-      <c r="K260" s="18"/>
-      <c r="L260" s="18"/>
-      <c r="M260" s="9"/>
-      <c r="N260" s="18"/>
-      <c r="O260" s="9"/>
-      <c r="P260" s="9"/>
+      <c r="A260" s="6"/>
+      <c r="B260" s="6"/>
+      <c r="C260" s="6"/>
+      <c r="D260" s="6"/>
+      <c r="E260" s="6"/>
+      <c r="F260" s="8"/>
+      <c r="G260" s="8"/>
+      <c r="H260" s="8"/>
+      <c r="I260" s="8"/>
+      <c r="J260" s="8"/>
+      <c r="K260" s="8"/>
+      <c r="L260" s="8"/>
+      <c r="M260" s="6"/>
+      <c r="N260" s="8"/>
+      <c r="O260" s="6"/>
+      <c r="P260" s="6"/>
       <c r="Q260" s="9"/>
       <c r="R260" s="9"/>
       <c r="S260" s="9"/>
       <c r="T260" s="9"/>
     </row>
     <row r="261" spans="1:20">
-      <c r="B261" s="9"/>
-      <c r="C261" s="9"/>
-      <c r="D261" s="9"/>
-      <c r="E261" s="9"/>
-      <c r="F261" s="18"/>
-      <c r="G261" s="18"/>
-      <c r="H261" s="18"/>
-      <c r="I261" s="18"/>
-      <c r="J261" s="18"/>
-      <c r="K261" s="18"/>
-      <c r="L261" s="18"/>
-      <c r="M261" s="9"/>
-      <c r="N261" s="18"/>
-      <c r="O261" s="9"/>
-      <c r="P261" s="9"/>
+      <c r="A261" s="6"/>
+      <c r="B261" s="6"/>
+      <c r="C261" s="6"/>
+      <c r="D261" s="6"/>
+      <c r="E261" s="6"/>
+      <c r="F261" s="8"/>
+      <c r="G261" s="8"/>
+      <c r="H261" s="8"/>
+      <c r="I261" s="8"/>
+      <c r="J261" s="8"/>
+      <c r="K261" s="8"/>
+      <c r="L261" s="8"/>
+      <c r="M261" s="6"/>
+      <c r="N261" s="8"/>
+      <c r="O261" s="6"/>
+      <c r="P261" s="6"/>
       <c r="Q261" s="9"/>
       <c r="R261" s="9"/>
       <c r="S261" s="9"/>
       <c r="T261" s="9"/>
     </row>
     <row r="262" spans="1:20">
-      <c r="B262" s="9"/>
-      <c r="C262" s="9"/>
-      <c r="D262" s="9"/>
-      <c r="E262" s="9"/>
-      <c r="F262" s="18"/>
-      <c r="G262" s="18"/>
-      <c r="H262" s="18"/>
-      <c r="I262" s="18"/>
-      <c r="J262" s="18"/>
-      <c r="K262" s="18"/>
-      <c r="L262" s="18"/>
-      <c r="M262" s="9"/>
-      <c r="N262" s="18"/>
-      <c r="O262" s="9"/>
-      <c r="P262" s="9"/>
+      <c r="A262" s="6"/>
+      <c r="B262" s="6"/>
+      <c r="C262" s="6"/>
+      <c r="D262" s="6"/>
+      <c r="E262" s="6"/>
+      <c r="F262" s="8"/>
+      <c r="G262" s="8"/>
+      <c r="H262" s="8"/>
+      <c r="I262" s="8"/>
+      <c r="J262" s="8"/>
+      <c r="K262" s="8"/>
+      <c r="L262" s="8"/>
+      <c r="M262" s="6"/>
+      <c r="N262" s="8"/>
+      <c r="O262" s="6"/>
+      <c r="P262" s="6"/>
       <c r="Q262" s="9"/>
       <c r="R262" s="9"/>
       <c r="S262" s="9"/>
       <c r="T262" s="9"/>
     </row>
     <row r="263" spans="1:20">
-      <c r="B263" s="9"/>
-      <c r="C263" s="9"/>
-      <c r="D263" s="9"/>
-      <c r="E263" s="9"/>
-      <c r="F263" s="18"/>
-      <c r="G263" s="18"/>
-      <c r="H263" s="18"/>
-      <c r="I263" s="18"/>
-      <c r="J263" s="18"/>
-      <c r="K263" s="18"/>
-      <c r="L263" s="18"/>
-      <c r="M263" s="9"/>
-      <c r="N263" s="18"/>
-      <c r="O263" s="9"/>
-      <c r="P263" s="9"/>
+      <c r="A263" s="6"/>
+      <c r="B263" s="6"/>
+      <c r="C263" s="6"/>
+      <c r="D263" s="6"/>
+      <c r="E263" s="6"/>
+      <c r="F263" s="8"/>
+      <c r="G263" s="8"/>
+      <c r="H263" s="8"/>
+      <c r="I263" s="8"/>
+      <c r="J263" s="8"/>
+      <c r="K263" s="8"/>
+      <c r="L263" s="8"/>
+      <c r="M263" s="6"/>
+      <c r="N263" s="8"/>
+      <c r="O263" s="6"/>
+      <c r="P263" s="6"/>
       <c r="Q263" s="9"/>
       <c r="R263" s="9"/>
       <c r="S263" s="9"/>
       <c r="T263" s="9"/>
     </row>
     <row r="264" spans="1:20">
+      <c r="A264" s="6"/>
       <c r="B264" s="9"/>
-      <c r="C264" s="9"/>
-      <c r="D264" s="9"/>
-      <c r="E264" s="9"/>
-      <c r="F264" s="18"/>
-      <c r="G264" s="18"/>
-      <c r="H264" s="18"/>
-      <c r="I264" s="18"/>
-      <c r="J264" s="18"/>
-      <c r="K264" s="18"/>
-      <c r="L264" s="18"/>
-      <c r="M264" s="9"/>
-      <c r="N264" s="18"/>
-      <c r="O264" s="9"/>
-      <c r="P264" s="9"/>
+      <c r="C264" s="6"/>
+      <c r="D264" s="6"/>
+      <c r="E264" s="6"/>
+      <c r="F264" s="8"/>
+      <c r="G264" s="8"/>
+      <c r="H264" s="8"/>
+      <c r="I264" s="8"/>
+      <c r="J264" s="8"/>
+      <c r="K264" s="8"/>
+      <c r="L264" s="8"/>
+      <c r="M264" s="6"/>
+      <c r="N264" s="8"/>
+      <c r="O264" s="6"/>
+      <c r="P264" s="6"/>
       <c r="Q264" s="9"/>
       <c r="R264" s="9"/>
       <c r="S264" s="9"/>
       <c r="T264" s="9"/>
     </row>
     <row r="265" spans="1:20">
+      <c r="A265" s="6"/>
       <c r="B265" s="9"/>
       <c r="C265" s="9"/>
-      <c r="D265" s="9"/>
-      <c r="E265" s="9"/>
-      <c r="F265" s="18"/>
-      <c r="G265" s="18"/>
-      <c r="H265" s="18"/>
-      <c r="I265" s="18"/>
-      <c r="J265" s="18"/>
-      <c r="K265" s="18"/>
-      <c r="L265" s="18"/>
-      <c r="M265" s="9"/>
-      <c r="N265" s="18"/>
-      <c r="O265" s="9"/>
-      <c r="P265" s="9"/>
+      <c r="D265" s="6"/>
+      <c r="E265" s="6"/>
+      <c r="F265" s="8"/>
+      <c r="G265" s="8"/>
+      <c r="H265" s="8"/>
+      <c r="I265" s="8"/>
+      <c r="J265" s="8"/>
+      <c r="K265" s="8"/>
+      <c r="L265" s="8"/>
+      <c r="M265" s="6"/>
+      <c r="N265" s="8"/>
+      <c r="O265" s="6"/>
+      <c r="P265" s="6"/>
       <c r="Q265" s="9"/>
       <c r="R265" s="9"/>
       <c r="S265" s="9"/>
@@ -11924,7 +12276,7 @@
       <c r="K337" s="18"/>
       <c r="L337" s="18"/>
       <c r="M337" s="9"/>
-      <c r="N337" s="9"/>
+      <c r="N337" s="18"/>
       <c r="O337" s="9"/>
       <c r="P337" s="9"/>
       <c r="Q337" s="9"/>
@@ -11945,7 +12297,7 @@
       <c r="K338" s="18"/>
       <c r="L338" s="18"/>
       <c r="M338" s="9"/>
-      <c r="N338" s="9"/>
+      <c r="N338" s="18"/>
       <c r="O338" s="9"/>
       <c r="P338" s="9"/>
       <c r="Q338" s="9"/>
@@ -11966,7 +12318,7 @@
       <c r="K339" s="18"/>
       <c r="L339" s="18"/>
       <c r="M339" s="9"/>
-      <c r="N339" s="9"/>
+      <c r="N339" s="18"/>
       <c r="O339" s="9"/>
       <c r="P339" s="9"/>
       <c r="Q339" s="9"/>
@@ -11987,7 +12339,7 @@
       <c r="K340" s="18"/>
       <c r="L340" s="18"/>
       <c r="M340" s="9"/>
-      <c r="N340" s="9"/>
+      <c r="N340" s="18"/>
       <c r="O340" s="9"/>
       <c r="P340" s="9"/>
       <c r="Q340" s="9"/>
@@ -12008,7 +12360,7 @@
       <c r="K341" s="18"/>
       <c r="L341" s="18"/>
       <c r="M341" s="9"/>
-      <c r="N341" s="9"/>
+      <c r="N341" s="18"/>
       <c r="O341" s="9"/>
       <c r="P341" s="9"/>
       <c r="Q341" s="9"/>
@@ -12029,7 +12381,7 @@
       <c r="K342" s="18"/>
       <c r="L342" s="18"/>
       <c r="M342" s="9"/>
-      <c r="N342" s="9"/>
+      <c r="N342" s="18"/>
       <c r="O342" s="9"/>
       <c r="P342" s="9"/>
       <c r="Q342" s="9"/>
@@ -12080,16 +12432,17 @@
       <c r="T344" s="9"/>
     </row>
     <row r="345" spans="2:20">
+      <c r="B345" s="9"/>
       <c r="C345" s="9"/>
       <c r="D345" s="9"/>
       <c r="E345" s="9"/>
-      <c r="F345" s="9"/>
-      <c r="G345" s="9"/>
-      <c r="H345" s="9"/>
-      <c r="I345" s="9"/>
-      <c r="J345" s="9"/>
-      <c r="K345" s="9"/>
-      <c r="L345" s="9"/>
+      <c r="F345" s="18"/>
+      <c r="G345" s="18"/>
+      <c r="H345" s="18"/>
+      <c r="I345" s="18"/>
+      <c r="J345" s="18"/>
+      <c r="K345" s="18"/>
+      <c r="L345" s="18"/>
       <c r="M345" s="9"/>
       <c r="N345" s="9"/>
       <c r="O345" s="9"/>
@@ -12100,15 +12453,17 @@
       <c r="T345" s="9"/>
     </row>
     <row r="346" spans="2:20">
+      <c r="B346" s="9"/>
+      <c r="C346" s="9"/>
       <c r="D346" s="9"/>
       <c r="E346" s="9"/>
-      <c r="F346" s="9"/>
-      <c r="G346" s="9"/>
-      <c r="H346" s="9"/>
-      <c r="I346" s="9"/>
-      <c r="J346" s="9"/>
-      <c r="K346" s="9"/>
-      <c r="L346" s="9"/>
+      <c r="F346" s="18"/>
+      <c r="G346" s="18"/>
+      <c r="H346" s="18"/>
+      <c r="I346" s="18"/>
+      <c r="J346" s="18"/>
+      <c r="K346" s="18"/>
+      <c r="L346" s="18"/>
       <c r="M346" s="9"/>
       <c r="N346" s="9"/>
       <c r="O346" s="9"/>
@@ -12118,11 +12473,134 @@
       <c r="S346" s="9"/>
       <c r="T346" s="9"/>
     </row>
+    <row r="347" spans="2:20">
+      <c r="B347" s="9"/>
+      <c r="C347" s="9"/>
+      <c r="D347" s="9"/>
+      <c r="E347" s="9"/>
+      <c r="F347" s="18"/>
+      <c r="G347" s="18"/>
+      <c r="H347" s="18"/>
+      <c r="I347" s="18"/>
+      <c r="J347" s="18"/>
+      <c r="K347" s="18"/>
+      <c r="L347" s="18"/>
+      <c r="M347" s="9"/>
+      <c r="N347" s="9"/>
+      <c r="O347" s="9"/>
+      <c r="P347" s="9"/>
+      <c r="Q347" s="9"/>
+      <c r="R347" s="9"/>
+      <c r="S347" s="9"/>
+      <c r="T347" s="9"/>
+    </row>
+    <row r="348" spans="2:20">
+      <c r="B348" s="9"/>
+      <c r="C348" s="9"/>
+      <c r="D348" s="9"/>
+      <c r="E348" s="9"/>
+      <c r="F348" s="18"/>
+      <c r="G348" s="18"/>
+      <c r="H348" s="18"/>
+      <c r="I348" s="18"/>
+      <c r="J348" s="18"/>
+      <c r="K348" s="18"/>
+      <c r="L348" s="18"/>
+      <c r="M348" s="9"/>
+      <c r="N348" s="9"/>
+      <c r="O348" s="9"/>
+      <c r="P348" s="9"/>
+      <c r="Q348" s="9"/>
+      <c r="R348" s="9"/>
+      <c r="S348" s="9"/>
+      <c r="T348" s="9"/>
+    </row>
+    <row r="349" spans="2:20">
+      <c r="B349" s="9"/>
+      <c r="C349" s="9"/>
+      <c r="D349" s="9"/>
+      <c r="E349" s="9"/>
+      <c r="F349" s="18"/>
+      <c r="G349" s="18"/>
+      <c r="H349" s="18"/>
+      <c r="I349" s="18"/>
+      <c r="J349" s="18"/>
+      <c r="K349" s="18"/>
+      <c r="L349" s="18"/>
+      <c r="M349" s="9"/>
+      <c r="N349" s="9"/>
+      <c r="O349" s="9"/>
+      <c r="P349" s="9"/>
+      <c r="Q349" s="9"/>
+      <c r="R349" s="9"/>
+      <c r="S349" s="9"/>
+      <c r="T349" s="9"/>
+    </row>
+    <row r="350" spans="2:20">
+      <c r="B350" s="9"/>
+      <c r="C350" s="9"/>
+      <c r="D350" s="9"/>
+      <c r="E350" s="9"/>
+      <c r="F350" s="18"/>
+      <c r="G350" s="18"/>
+      <c r="H350" s="18"/>
+      <c r="I350" s="18"/>
+      <c r="J350" s="18"/>
+      <c r="K350" s="18"/>
+      <c r="L350" s="18"/>
+      <c r="M350" s="9"/>
+      <c r="N350" s="9"/>
+      <c r="O350" s="9"/>
+      <c r="P350" s="9"/>
+      <c r="Q350" s="9"/>
+      <c r="R350" s="9"/>
+      <c r="S350" s="9"/>
+      <c r="T350" s="9"/>
+    </row>
+    <row r="351" spans="2:20">
+      <c r="C351" s="9"/>
+      <c r="D351" s="9"/>
+      <c r="E351" s="9"/>
+      <c r="F351" s="9"/>
+      <c r="G351" s="9"/>
+      <c r="H351" s="9"/>
+      <c r="I351" s="9"/>
+      <c r="J351" s="9"/>
+      <c r="K351" s="9"/>
+      <c r="L351" s="9"/>
+      <c r="M351" s="9"/>
+      <c r="N351" s="9"/>
+      <c r="O351" s="9"/>
+      <c r="P351" s="9"/>
+      <c r="Q351" s="9"/>
+      <c r="R351" s="9"/>
+      <c r="S351" s="9"/>
+      <c r="T351" s="9"/>
+    </row>
+    <row r="352" spans="2:20">
+      <c r="D352" s="9"/>
+      <c r="E352" s="9"/>
+      <c r="F352" s="9"/>
+      <c r="G352" s="9"/>
+      <c r="H352" s="9"/>
+      <c r="I352" s="9"/>
+      <c r="J352" s="9"/>
+      <c r="K352" s="9"/>
+      <c r="L352" s="9"/>
+      <c r="M352" s="9"/>
+      <c r="N352" s="9"/>
+      <c r="O352" s="9"/>
+      <c r="P352" s="9"/>
+      <c r="Q352" s="9"/>
+      <c r="R352" s="9"/>
+      <c r="S352" s="9"/>
+      <c r="T352" s="9"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H20 H22:H55 H68:H1048576">
+  <conditionalFormatting sqref="H1:H20 H74:H1048576 H22:H61">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -12133,7 +12611,7 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H59:H63">
+  <conditionalFormatting sqref="H65:H69">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -12144,17 +12622,17 @@
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J20 J22:J64 J66 J68:J248">
+  <conditionalFormatting sqref="J7:J20 J72 J74:J254 J22:J70">
     <cfRule type="notContainsBlanks" dxfId="2" priority="724">
       <formula>LEN(TRIM(J7))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K17 K22:L38">
+  <conditionalFormatting sqref="K17 K22:L44">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(K17))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:L16 L18:L21 L39:L55 K40:K50 K56:K64 K62:L63 K66 K68:L248">
+  <conditionalFormatting sqref="K7:L16 L18:L21 L45:L61 K46:K56 K62:K70 K68:L69 K72 K74:L254">
     <cfRule type="notContainsBlanks" dxfId="0" priority="725">
       <formula>LEN(TRIM(K7))&gt;0</formula>
     </cfRule>
@@ -27720,16 +28198,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E329102-D1E6-314A-A75F-E468AE5BC4F5}">
-  <dimension ref="B2:N10"/>
+  <dimension ref="B1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
-    <col min="7" max="7" width="16" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="32"/>
+    <col min="7" max="7" width="16" style="32" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
@@ -27739,344 +28219,611 @@
     <col min="14" max="14" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
-      <c r="B2" s="57" t="s">
+    <row r="1" spans="2:14" ht="31">
+      <c r="B1" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C1" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D1" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="57" t="s">
+      <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="57" t="s">
+      <c r="F1" s="67" t="s">
         <v>120</v>
       </c>
-      <c r="G2" s="57" t="s">
+      <c r="G1" s="67" t="s">
         <v>106</v>
       </c>
-      <c r="H2" s="57" t="s">
+      <c r="H1" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="I2" s="57" t="s">
+      <c r="I1" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="57" t="s">
+      <c r="J1" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="K2" s="57" t="s">
+      <c r="K1" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="L2" s="57" t="s">
+      <c r="L1" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="M2" s="57" t="s">
-        <v>144</v>
-      </c>
-      <c r="N2" s="57" t="s">
+      <c r="M1" s="30" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="3" spans="2:14" ht="63" customHeight="1">
+      <c r="N1" s="30" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="2:14" ht="63" customHeight="1">
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2020</v>
+      </c>
+      <c r="F2" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="69" t="s">
+        <v>118</v>
+      </c>
+      <c r="M2" s="69"/>
+      <c r="N2" s="21"/>
+    </row>
+    <row r="3" spans="2:14" ht="61">
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E3" s="8">
         <v>2020</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="58" t="s">
+      <c r="G3" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I3" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="H3" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="I3" s="58" t="s">
-        <v>110</v>
-      </c>
-      <c r="J3" s="58" t="s">
-        <v>115</v>
-      </c>
-      <c r="K3" s="59" t="s">
+      <c r="J3" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="60" t="s">
-        <v>118</v>
-      </c>
-      <c r="M3" s="60"/>
-    </row>
-    <row r="4" spans="2:14" ht="64">
+      <c r="L3" s="69" t="s">
+        <v>119</v>
+      </c>
+      <c r="M3" s="69"/>
+      <c r="N3" s="21"/>
+    </row>
+    <row r="4" spans="2:14" ht="91">
       <c r="B4" s="6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="8">
-        <v>2020</v>
-      </c>
-      <c r="F4" s="8" t="s">
+        <v>2021</v>
+      </c>
+      <c r="F4" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" s="6"/>
+      <c r="N4" s="31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" ht="61">
+      <c r="B5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F5" s="64" t="s">
+        <v>126</v>
+      </c>
+      <c r="G5" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="K5" s="69" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="M5" s="69"/>
+      <c r="N5" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" ht="46">
+      <c r="B6" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="34">
+        <v>2022</v>
+      </c>
+      <c r="F6" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="G4" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="H4" s="58" t="s">
+      <c r="G6" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="I4" s="58" t="s">
+      <c r="I6" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="60" t="s">
+      <c r="K6" s="69" t="s">
+        <v>129</v>
+      </c>
+      <c r="L6" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="M6" s="69"/>
+      <c r="N6" s="21"/>
+    </row>
+    <row r="7" spans="2:14" ht="61">
+      <c r="B7" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2022</v>
+      </c>
+      <c r="F7" s="64" t="s">
+        <v>141</v>
+      </c>
+      <c r="G7" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="J7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="K7" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="L4" s="60" t="s">
-        <v>119</v>
-      </c>
-      <c r="M4" s="60"/>
-    </row>
-    <row r="5" spans="2:14" ht="96">
-      <c r="B5" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="8">
-        <v>2021</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="G5" s="58" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="58" t="s">
-        <v>139</v>
-      </c>
-      <c r="I5" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" t="s">
-        <v>116</v>
-      </c>
-      <c r="K5" s="60" t="s">
-        <v>122</v>
-      </c>
-      <c r="L5" s="58" t="s">
-        <v>123</v>
-      </c>
-      <c r="M5" s="58"/>
-      <c r="N5" s="59" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="2:14" ht="64">
-      <c r="B6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="8">
-        <v>2022</v>
-      </c>
-      <c r="F6" s="61" t="s">
-        <v>128</v>
-      </c>
-      <c r="G6" s="58" t="s">
-        <v>126</v>
-      </c>
-      <c r="H6" s="58" t="s">
+      <c r="L7" s="69" t="s">
+        <v>147</v>
+      </c>
+      <c r="M7" s="69"/>
+      <c r="N7" s="21"/>
+    </row>
+    <row r="8" spans="2:14" ht="76">
+      <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E8" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F8" s="64" t="s">
+        <v>143</v>
+      </c>
+      <c r="G8" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="H8" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="I6" s="58" t="s">
-        <v>129</v>
-      </c>
-      <c r="J6" s="58" t="s">
-        <v>116</v>
-      </c>
-      <c r="K6" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="L6" s="60" t="s">
-        <v>130</v>
-      </c>
-      <c r="M6" s="60"/>
-      <c r="N6" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="7" spans="2:14" ht="48">
-      <c r="B7" s="62" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="62" t="s">
-        <v>45</v>
-      </c>
-      <c r="D7" s="62" t="s">
-        <v>59</v>
-      </c>
-      <c r="E7" s="63">
-        <v>2022</v>
-      </c>
-      <c r="F7" s="61" t="s">
+      <c r="I8" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="J8" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="K8" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="69" t="s">
+        <v>146</v>
+      </c>
+      <c r="M8" s="69" t="s">
+        <v>148</v>
+      </c>
+      <c r="N8" s="21"/>
+    </row>
+    <row r="9" spans="2:14" ht="76">
+      <c r="B9" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F9" s="64" t="s">
         <v>121</v>
       </c>
-      <c r="G7" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>140</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="J7" t="s">
-        <v>116</v>
-      </c>
-      <c r="K7" s="60" t="s">
+      <c r="G9" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="L7" s="60" t="s">
-        <v>132</v>
-      </c>
-      <c r="M7" s="60"/>
-    </row>
-    <row r="8" spans="2:14" ht="64">
-      <c r="B8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="8">
-        <v>2022</v>
-      </c>
-      <c r="F8" s="61" t="s">
-        <v>143</v>
-      </c>
-      <c r="G8" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="H8" s="58" t="s">
-        <v>138</v>
-      </c>
-      <c r="I8" s="58" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" t="s">
-        <v>116</v>
-      </c>
-      <c r="K8" s="60" t="s">
-        <v>117</v>
-      </c>
-      <c r="L8" s="60" t="s">
+      <c r="H9" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="K9" s="69" t="s">
+        <v>150</v>
+      </c>
+      <c r="L9" s="69" t="s">
         <v>149</v>
       </c>
-      <c r="M8" s="60"/>
-    </row>
-    <row r="9" spans="2:14" ht="80">
-      <c r="B9" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="M9" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="2:14" ht="76">
+      <c r="B10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2023</v>
-      </c>
-      <c r="F9" s="61" t="s">
-        <v>145</v>
-      </c>
-      <c r="G9" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="H9" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="58" t="s">
-        <v>147</v>
-      </c>
-      <c r="J9" t="s">
-        <v>154</v>
-      </c>
-      <c r="K9" s="60" t="s">
-        <v>146</v>
-      </c>
-      <c r="L9" s="60" t="s">
-        <v>148</v>
-      </c>
-      <c r="M9" s="60" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="80">
-      <c r="B10" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="E10" s="8">
         <v>2024</v>
       </c>
-      <c r="F10" s="61" t="s">
-        <v>121</v>
-      </c>
-      <c r="G10" s="62" t="s">
-        <v>133</v>
-      </c>
-      <c r="H10" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" s="58" t="s">
-        <v>137</v>
-      </c>
-      <c r="J10" t="s">
-        <v>154</v>
-      </c>
-      <c r="K10" s="60" t="s">
+      <c r="F10" s="65" t="s">
         <v>153</v>
       </c>
-      <c r="L10" s="60" t="s">
+      <c r="G10" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="M10" t="s">
-        <v>151</v>
-      </c>
+      <c r="H10" s="63" t="s">
+        <v>155</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="J10" s="70" t="s">
+        <v>157</v>
+      </c>
+      <c r="K10" s="69" t="s">
+        <v>159</v>
+      </c>
+      <c r="L10" s="69" t="s">
+        <v>161</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="2:14" ht="106">
+      <c r="B11" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="E11" s="8">
+        <v>2023</v>
+      </c>
+      <c r="F11" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G11" s="66" t="s">
+        <v>131</v>
+      </c>
+      <c r="H11" s="68" t="s">
+        <v>168</v>
+      </c>
+      <c r="I11" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J11" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K11" s="69" t="s">
+        <v>184</v>
+      </c>
+      <c r="L11" s="69" t="s">
+        <v>169</v>
+      </c>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+    </row>
+    <row r="12" spans="2:14" ht="121">
+      <c r="B12" s="21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C12" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>173</v>
+      </c>
+      <c r="E12" s="62">
+        <v>2021</v>
+      </c>
+      <c r="F12" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="G12" s="69" t="s">
+        <v>176</v>
+      </c>
+      <c r="H12" s="68" t="s">
+        <v>175</v>
+      </c>
+      <c r="I12" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="69" t="s">
+        <v>177</v>
+      </c>
+      <c r="L12" s="69" t="s">
+        <v>170</v>
+      </c>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+    </row>
+    <row r="13" spans="2:14" ht="106">
+      <c r="B13" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="E13" s="8">
+        <v>2012</v>
+      </c>
+      <c r="F13" s="65" t="s">
+        <v>167</v>
+      </c>
+      <c r="G13" s="66" t="s">
+        <v>183</v>
+      </c>
+      <c r="H13" s="63" t="s">
+        <v>185</v>
+      </c>
+      <c r="I13" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J13" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K13" s="69" t="s">
+        <v>191</v>
+      </c>
+      <c r="L13" s="69" t="s">
+        <v>186</v>
+      </c>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+    </row>
+    <row r="14" spans="2:14" ht="166">
+      <c r="B14" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="62">
+        <v>2021</v>
+      </c>
+      <c r="F14" s="69" t="s">
+        <v>193</v>
+      </c>
+      <c r="G14" s="69" t="s">
+        <v>190</v>
+      </c>
+      <c r="H14" s="68" t="s">
+        <v>195</v>
+      </c>
+      <c r="I14" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K14" s="69" t="s">
+        <v>192</v>
+      </c>
+      <c r="L14" s="69" t="s">
+        <v>194</v>
+      </c>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+    </row>
+    <row r="15" spans="2:14" ht="61">
+      <c r="B15" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2020</v>
+      </c>
+      <c r="F15" s="69" t="s">
+        <v>199</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>198</v>
+      </c>
+      <c r="H15" s="68" t="s">
+        <v>200</v>
+      </c>
+      <c r="I15" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J15" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K15" s="69" t="s">
+        <v>201</v>
+      </c>
+      <c r="L15" s="69" t="s">
+        <v>202</v>
+      </c>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+    </row>
+    <row r="16" spans="2:14" ht="136">
+      <c r="B16" s="63" t="s">
+        <v>203</v>
+      </c>
+      <c r="C16" s="63" t="s">
+        <v>204</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="62">
+        <v>2024</v>
+      </c>
+      <c r="F16" s="69" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="69" t="s">
+        <v>206</v>
+      </c>
+      <c r="H16" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="I16" s="63" t="s">
+        <v>115</v>
+      </c>
+      <c r="J16" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="69" t="s">
+        <v>208</v>
+      </c>
+      <c r="L16" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adjusted literature review table
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FAC372-3AF5-484F-92AB-677C94082D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{604F2D7C-D3FC-E645-8BFE-1E478CF72093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="3" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
@@ -863,9 +863,6 @@
     <t>IEEE Transactions on Industrial Electronics</t>
   </si>
   <si>
-    <t>Minimize generation cost+start-up+shut down</t>
-  </si>
-  <si>
     <t>Generation availability
 Load balance
 Voltage violation
@@ -947,6 +944,9 @@
   </si>
   <si>
     <t xml:space="preserve">Pg, Vg, Ttrfo, </t>
+  </si>
+  <si>
+    <t>Minimize generation +start-up+shut down cost</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1299,8 +1299,60 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1317,9 +1369,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1335,74 +1384,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1451,21 +1441,21 @@
     </dxf>
     <dxf>
       <font>
+        <color theme="5"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2778,23 +2768,23 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="47"/>
-      <c r="G2" s="48"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="42"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="55"/>
+      <c r="K2" s="44"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="35" t="s">
+      <c r="M2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="47"/>
-      <c r="O2" s="48"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="42"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="55"/>
+      <c r="Q2" s="44"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2823,19 +2813,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="56"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="45"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="41"/>
+      <c r="K3" s="49"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="55"/>
-      <c r="O3" s="56"/>
+      <c r="M3" s="43"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="45"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="41"/>
+      <c r="Q3" s="49"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2864,19 +2854,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="50"/>
-      <c r="G4" s="51"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="48"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="41"/>
+      <c r="K4" s="49"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="50"/>
-      <c r="O4" s="51"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="47"/>
+      <c r="O4" s="48"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="41"/>
+      <c r="Q4" s="49"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -3027,15 +3017,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="50" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="50" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="59" t="s">
+      <c r="H8" s="52" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -3074,11 +3064,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="58"/>
+      <c r="D9" s="51"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="58"/>
+      <c r="F9" s="51"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="60"/>
+      <c r="H9" s="53"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -3201,18 +3191,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="42" t="s">
+      <c r="H12" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="61"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="42" t="s">
+      <c r="M12" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="45"/>
-      <c r="O12" s="46"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="63"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -3328,18 +3318,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="42" t="s">
+      <c r="H15" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="61"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="42" t="s">
+      <c r="M15" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="44"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -3455,18 +3445,18 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="35" t="s">
+      <c r="H18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="47"/>
-      <c r="J18" s="48"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="42"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="35" t="s">
+      <c r="M18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37"/>
+      <c r="N18" s="54"/>
+      <c r="O18" s="55"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3500,14 +3490,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="50"/>
-      <c r="J19" s="51"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="48"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="39"/>
-      <c r="O19" s="40"/>
+      <c r="M19" s="56"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="58"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3623,11 +3613,11 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="37"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="55"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3666,9 +3656,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="40"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3747,10 +3737,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="52" t="s">
+      <c r="G25" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="53"/>
+      <c r="H25" s="65"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
         <v>19</v>
@@ -3871,8 +3861,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -4402,13 +4392,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="M2:O4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H22:J23"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="H12:J12"/>
@@ -4418,6 +4401,13 @@
     <mergeCell ref="H18:J19"/>
     <mergeCell ref="M18:O19"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E2:G4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:O4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4487,10 +4477,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="61" t="s">
+      <c r="J2" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="61"/>
+      <c r="K2" s="66"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>34</v>
@@ -5697,13 +5687,13 @@
       <c r="C38" t="s">
         <v>171</v>
       </c>
-      <c r="D38" s="63" t="s">
+      <c r="D38" s="6" t="s">
         <v>172</v>
       </c>
       <c r="E38" t="s">
         <v>173</v>
       </c>
-      <c r="F38" s="62">
+      <c r="F38" s="8">
         <v>2021</v>
       </c>
       <c r="G38" s="8"/>
@@ -5802,7 +5792,7 @@
       <c r="B41" s="12">
         <v>28</v>
       </c>
-      <c r="C41" s="63" t="s">
+      <c r="C41" s="6" t="s">
         <v>187</v>
       </c>
       <c r="D41" t="s">
@@ -5811,7 +5801,7 @@
       <c r="E41" t="s">
         <v>189</v>
       </c>
-      <c r="F41" s="62">
+      <c r="F41" s="8">
         <v>2021</v>
       </c>
       <c r="G41" s="8"/>
@@ -5839,10 +5829,10 @@
         <v>29</v>
       </c>
       <c r="C42" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="D42" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>82</v>
@@ -5874,16 +5864,16 @@
       <c r="B43" s="12">
         <v>30</v>
       </c>
-      <c r="C43" s="63" t="s">
+      <c r="C43" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="D43" s="63" t="s">
+      <c r="E43" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="E43" s="21" t="s">
-        <v>205</v>
-      </c>
-      <c r="F43" s="62">
+      <c r="F43" s="8">
         <v>2024</v>
       </c>
       <c r="G43" s="8"/>
@@ -12600,7 +12590,7 @@
   <mergeCells count="1">
     <mergeCell ref="J2:K2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H1:H20 H74:H1048576 H22:H61">
+  <conditionalFormatting sqref="H1:H20 H22:H61 H74:H1048576">
     <cfRule type="cellIs" dxfId="8" priority="5" operator="equal">
       <formula>"M"</formula>
     </cfRule>
@@ -12612,17 +12602,17 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H65:H69">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
       <formula>"M"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
-      <formula>"N"</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J20 J72 J74:J254 J22:J70">
+  <conditionalFormatting sqref="J7:J20 J22:J70 J72 J74:J254">
     <cfRule type="notContainsBlanks" dxfId="2" priority="724">
       <formula>LEN(TRIM(J7))&gt;0</formula>
     </cfRule>
@@ -28201,8 +28191,8 @@
   <dimension ref="B1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L27" sqref="L27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -28232,10 +28222,10 @@
       <c r="E1" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="67" t="s">
+      <c r="F1" s="37" t="s">
         <v>120</v>
       </c>
-      <c r="G1" s="67" t="s">
+      <c r="G1" s="37" t="s">
         <v>106</v>
       </c>
       <c r="H1" s="30" t="s">
@@ -28273,7 +28263,7 @@
       <c r="E2" s="8">
         <v>2020</v>
       </c>
-      <c r="F2" s="64" t="s">
+      <c r="F2" s="35" t="s">
         <v>121</v>
       </c>
       <c r="G2" s="31" t="s">
@@ -28291,10 +28281,10 @@
       <c r="K2" s="31" t="s">
         <v>117</v>
       </c>
-      <c r="L2" s="69" t="s">
+      <c r="L2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="M2" s="69"/>
+      <c r="M2" s="38"/>
       <c r="N2" s="21"/>
     </row>
     <row r="3" spans="2:14" ht="61">
@@ -28310,7 +28300,7 @@
       <c r="E3" s="8">
         <v>2020</v>
       </c>
-      <c r="F3" s="64" t="s">
+      <c r="F3" s="35" t="s">
         <v>121</v>
       </c>
       <c r="G3" s="31" t="s">
@@ -28325,13 +28315,13 @@
       <c r="J3" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="K3" s="69" t="s">
+      <c r="K3" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="69" t="s">
+      <c r="L3" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="M3" s="69"/>
+      <c r="M3" s="38"/>
       <c r="N3" s="21"/>
     </row>
     <row r="4" spans="2:14" ht="91">
@@ -28347,7 +28337,7 @@
       <c r="E4" s="8">
         <v>2021</v>
       </c>
-      <c r="F4" s="64" t="s">
+      <c r="F4" s="35" t="s">
         <v>154</v>
       </c>
       <c r="G4" s="31" t="s">
@@ -28362,7 +28352,7 @@
       <c r="J4" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="69" t="s">
+      <c r="K4" s="38" t="s">
         <v>158</v>
       </c>
       <c r="L4" s="6" t="s">
@@ -28386,7 +28376,7 @@
       <c r="E5" s="8">
         <v>2022</v>
       </c>
-      <c r="F5" s="64" t="s">
+      <c r="F5" s="35" t="s">
         <v>126</v>
       </c>
       <c r="G5" s="31" t="s">
@@ -28401,13 +28391,13 @@
       <c r="J5" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="K5" s="69" t="s">
+      <c r="K5" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="M5" s="69"/>
+      <c r="M5" s="38"/>
       <c r="N5" s="21" t="s">
         <v>124</v>
       </c>
@@ -28425,10 +28415,10 @@
       <c r="E6" s="34">
         <v>2022</v>
       </c>
-      <c r="F6" s="64" t="s">
+      <c r="F6" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="G6" s="66" t="s">
+      <c r="G6" s="36" t="s">
         <v>131</v>
       </c>
       <c r="H6" s="6" t="s">
@@ -28440,13 +28430,13 @@
       <c r="J6" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="K6" s="69" t="s">
+      <c r="K6" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="L6" s="69" t="s">
+      <c r="L6" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="M6" s="69"/>
+      <c r="M6" s="38"/>
       <c r="N6" s="21"/>
     </row>
     <row r="7" spans="2:14" ht="61">
@@ -28462,10 +28452,10 @@
       <c r="E7" s="8">
         <v>2022</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="G7" s="66" t="s">
+      <c r="G7" s="36" t="s">
         <v>131</v>
       </c>
       <c r="H7" s="6" t="s">
@@ -28477,13 +28467,13 @@
       <c r="J7" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="K7" s="69" t="s">
+      <c r="K7" s="38" t="s">
         <v>117</v>
       </c>
-      <c r="L7" s="69" t="s">
+      <c r="L7" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="M7" s="69"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="21"/>
     </row>
     <row r="8" spans="2:14" ht="76">
@@ -28499,10 +28489,10 @@
       <c r="E8" s="8">
         <v>2023</v>
       </c>
-      <c r="F8" s="64" t="s">
+      <c r="F8" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="G8" s="66" t="s">
+      <c r="G8" s="36" t="s">
         <v>131</v>
       </c>
       <c r="H8" s="6" t="s">
@@ -28514,13 +28504,13 @@
       <c r="J8" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="K8" s="69" t="s">
+      <c r="K8" s="38" t="s">
         <v>144</v>
       </c>
-      <c r="L8" s="69" t="s">
+      <c r="L8" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="69" t="s">
+      <c r="M8" s="38" t="s">
         <v>148</v>
       </c>
       <c r="N8" s="21"/>
@@ -28538,10 +28528,10 @@
       <c r="E9" s="8">
         <v>2024</v>
       </c>
-      <c r="F9" s="64" t="s">
+      <c r="F9" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="66" t="s">
+      <c r="G9" s="36" t="s">
         <v>131</v>
       </c>
       <c r="H9" s="6" t="s">
@@ -28553,10 +28543,10 @@
       <c r="J9" s="21" t="s">
         <v>151</v>
       </c>
-      <c r="K9" s="69" t="s">
+      <c r="K9" s="38" t="s">
         <v>150</v>
       </c>
-      <c r="L9" s="69" t="s">
+      <c r="L9" s="38" t="s">
         <v>149</v>
       </c>
       <c r="M9" s="21" t="s">
@@ -28577,25 +28567,25 @@
       <c r="E10" s="8">
         <v>2024</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="36" t="s">
         <v>152</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="H10" s="6" t="s">
         <v>155</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="J10" s="70" t="s">
+      <c r="J10" s="39" t="s">
         <v>157</v>
       </c>
-      <c r="K10" s="69" t="s">
+      <c r="K10" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="L10" s="69" t="s">
+      <c r="L10" s="38" t="s">
         <v>161</v>
       </c>
       <c r="M10" s="21" t="s">
@@ -28616,25 +28606,25 @@
       <c r="E11" s="8">
         <v>2023</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="36" t="s">
         <v>131</v>
       </c>
-      <c r="H11" s="68" t="s">
+      <c r="H11" s="31" t="s">
         <v>168</v>
       </c>
-      <c r="I11" s="63" t="s">
+      <c r="I11" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J11" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K11" s="69" t="s">
+      <c r="K11" s="38" t="s">
         <v>184</v>
       </c>
-      <c r="L11" s="69" t="s">
+      <c r="L11" s="38" t="s">
         <v>169</v>
       </c>
       <c r="M11" s="21"/>
@@ -28644,34 +28634,34 @@
       <c r="B12" s="21" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="6" t="s">
         <v>172</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="62">
+      <c r="E12" s="8">
         <v>2021</v>
       </c>
-      <c r="F12" s="69" t="s">
+      <c r="F12" s="38" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="38" t="s">
         <v>176</v>
       </c>
-      <c r="H12" s="68" t="s">
+      <c r="H12" s="31" t="s">
         <v>175</v>
       </c>
-      <c r="I12" s="63" t="s">
+      <c r="I12" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J12" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K12" s="69" t="s">
+      <c r="K12" s="38" t="s">
         <v>177</v>
       </c>
-      <c r="L12" s="69" t="s">
+      <c r="L12" s="38" t="s">
         <v>170</v>
       </c>
       <c r="M12" s="21"/>
@@ -28690,32 +28680,32 @@
       <c r="E13" s="8">
         <v>2012</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="G13" s="66" t="s">
+      <c r="G13" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="H13" s="63" t="s">
+      <c r="H13" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="I13" s="63" t="s">
+      <c r="I13" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J13" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K13" s="69" t="s">
-        <v>191</v>
-      </c>
-      <c r="L13" s="69" t="s">
+      <c r="K13" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="L13" s="38" t="s">
         <v>186</v>
       </c>
       <c r="M13" s="21"/>
       <c r="N13" s="21"/>
     </row>
     <row r="14" spans="2:14" ht="166">
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="6" t="s">
         <v>187</v>
       </c>
       <c r="C14" s="21" t="s">
@@ -28724,39 +28714,39 @@
       <c r="D14" s="21" t="s">
         <v>189</v>
       </c>
-      <c r="E14" s="62">
+      <c r="E14" s="8">
         <v>2021</v>
       </c>
-      <c r="F14" s="69" t="s">
-        <v>193</v>
-      </c>
-      <c r="G14" s="69" t="s">
-        <v>190</v>
-      </c>
-      <c r="H14" s="68" t="s">
-        <v>195</v>
-      </c>
-      <c r="I14" s="63" t="s">
+      <c r="F14" s="38" t="s">
+        <v>192</v>
+      </c>
+      <c r="G14" s="38" t="s">
+        <v>210</v>
+      </c>
+      <c r="H14" s="31" t="s">
+        <v>194</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J14" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K14" s="69" t="s">
-        <v>192</v>
-      </c>
-      <c r="L14" s="69" t="s">
-        <v>194</v>
+      <c r="K14" s="38" t="s">
+        <v>191</v>
+      </c>
+      <c r="L14" s="38" t="s">
+        <v>193</v>
       </c>
       <c r="M14" s="21"/>
       <c r="N14" s="21"/>
     </row>
     <row r="15" spans="2:14" ht="61">
       <c r="B15" s="6" t="s">
+        <v>195</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>82</v>
@@ -28764,63 +28754,63 @@
       <c r="E15" s="8">
         <v>2020</v>
       </c>
-      <c r="F15" s="69" t="s">
+      <c r="F15" s="38" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="38" t="s">
+        <v>197</v>
+      </c>
+      <c r="H15" s="31" t="s">
         <v>199</v>
       </c>
-      <c r="G15" s="69" t="s">
-        <v>198</v>
-      </c>
-      <c r="H15" s="68" t="s">
-        <v>200</v>
-      </c>
-      <c r="I15" s="63" t="s">
+      <c r="I15" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J15" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K15" s="69" t="s">
+      <c r="K15" s="38" t="s">
+        <v>200</v>
+      </c>
+      <c r="L15" s="38" t="s">
         <v>201</v>
-      </c>
-      <c r="L15" s="69" t="s">
-        <v>202</v>
       </c>
       <c r="M15" s="21"/>
       <c r="N15" s="21"/>
     </row>
     <row r="16" spans="2:14" ht="136">
-      <c r="B16" s="63" t="s">
+      <c r="B16" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="C16" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="C16" s="63" t="s">
+      <c r="D16" s="21" t="s">
         <v>204</v>
       </c>
-      <c r="D16" s="21" t="s">
+      <c r="E16" s="8">
+        <v>2024</v>
+      </c>
+      <c r="F16" s="38" t="s">
+        <v>208</v>
+      </c>
+      <c r="G16" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="E16" s="62">
-        <v>2024</v>
-      </c>
-      <c r="F16" s="69" t="s">
+      <c r="H16" s="21" t="s">
         <v>209</v>
       </c>
-      <c r="G16" s="69" t="s">
-        <v>206</v>
-      </c>
-      <c r="H16" s="21" t="s">
-        <v>210</v>
-      </c>
-      <c r="I16" s="63" t="s">
+      <c r="I16" s="6" t="s">
         <v>115</v>
       </c>
       <c r="J16" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="K16" s="69" t="s">
-        <v>208</v>
+      <c r="K16" s="38" t="s">
+        <v>207</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="M16" s="21"/>
       <c r="N16" s="21"/>

</xml_diff>

<commit_message>
created A-C Framework image
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702061F0-2DE1-E24C-B9CE-FC334292786E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D5D8A5-A86A-334D-BBD1-5B606424BBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
+    <workbookView xWindow="32880" yWindow="1540" windowWidth="28800" windowHeight="15800" activeTab="3" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
   <sheets>
     <sheet name="Four-phase flow diagram" sheetId="2" r:id="rId1"/>
@@ -1320,7 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -1416,45 +1416,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1469,6 +1430,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1485,17 +1449,49 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2876,20 +2872,20 @@
       <c r="E2" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="41"/>
-      <c r="G2" s="42"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="53"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="44"/>
+      <c r="K2" s="60"/>
       <c r="L2" s="1"/>
       <c r="M2" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="42"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="53"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="44"/>
+      <c r="Q2" s="60"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -2918,19 +2914,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="45"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="60"/>
+      <c r="G3" s="61"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="49"/>
+      <c r="K3" s="46"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="43"/>
-      <c r="N3" s="44"/>
-      <c r="O3" s="45"/>
+      <c r="M3" s="59"/>
+      <c r="N3" s="60"/>
+      <c r="O3" s="61"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="49"/>
+      <c r="Q3" s="46"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -2959,19 +2955,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="55"/>
+      <c r="G4" s="56"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="49"/>
+      <c r="K4" s="46"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="46"/>
-      <c r="N4" s="47"/>
-      <c r="O4" s="48"/>
+      <c r="M4" s="54"/>
+      <c r="N4" s="55"/>
+      <c r="O4" s="56"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="49"/>
+      <c r="Q4" s="46"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -3122,15 +3118,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="50" t="s">
+      <c r="D8" s="62" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="50" t="s">
+      <c r="F8" s="62" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="52" t="s">
+      <c r="H8" s="64" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -3169,11 +3165,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="51"/>
+      <c r="D9" s="63"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="51"/>
+      <c r="F9" s="63"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="53"/>
+      <c r="H9" s="65"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -3296,18 +3292,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="59" t="s">
+      <c r="H12" s="47" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="60"/>
-      <c r="J12" s="61"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="49"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="59" t="s">
+      <c r="M12" s="47" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="62"/>
-      <c r="O12" s="63"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="51"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -3423,18 +3419,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="59" t="s">
+      <c r="H15" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="60"/>
-      <c r="J15" s="61"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="49"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="59" t="s">
+      <c r="M15" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="60"/>
-      <c r="O15" s="61"/>
+      <c r="N15" s="48"/>
+      <c r="O15" s="49"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -3553,15 +3549,15 @@
       <c r="H18" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="41"/>
-      <c r="J18" s="42"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="53"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="54"/>
-      <c r="O18" s="55"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="42"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3595,14 +3591,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="54"/>
+      <c r="I19" s="55"/>
+      <c r="J19" s="56"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="58"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="44"/>
+      <c r="O19" s="45"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3721,8 +3717,8 @@
       <c r="H22" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="42"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3761,9 +3757,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="57"/>
-      <c r="J23" s="58"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="45"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3842,10 +3838,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="64" t="s">
+      <c r="G25" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="65"/>
+      <c r="H25" s="58"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
         <v>19</v>
@@ -3966,8 +3962,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
+      <c r="D28" s="46"/>
+      <c r="E28" s="46"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -4497,6 +4493,13 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="E2:G4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:O4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H22:J23"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="H12:J12"/>
@@ -4506,13 +4509,6 @@
     <mergeCell ref="H18:J19"/>
     <mergeCell ref="M18:O19"/>
     <mergeCell ref="G25:H25"/>
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="M2:O4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -28295,20 +28291,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E329102-D1E6-314A-A75F-E468AE5BC4F5}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
+    <col min="2" max="2" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="7.83203125" customWidth="1"/>
     <col min="6" max="6" width="10.83203125" style="32"/>
     <col min="7" max="7" width="16" style="32" customWidth="1"/>
     <col min="8" max="8" width="16.33203125" customWidth="1"/>
     <col min="9" max="9" width="17.33203125" customWidth="1"/>
     <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="29.33203125" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" customWidth="1"/>
     <col min="12" max="12" width="56.5" customWidth="1"/>
     <col min="13" max="13" width="14.5" customWidth="1"/>
     <col min="14" max="14" width="16.33203125" customWidth="1"/>
@@ -29066,16 +29063,16 @@
       </c>
     </row>
     <row r="22" spans="1:14" ht="32">
-      <c r="B22" s="67" t="s">
+      <c r="B22" s="6" t="s">
         <v>238</v>
       </c>
       <c r="C22" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="D22" s="67" t="s">
+      <c r="D22" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="68">
+      <c r="E22" s="8">
         <v>2012</v>
       </c>
       <c r="F22" s="32" t="s">
@@ -29089,16 +29086,16 @@
       </c>
     </row>
     <row r="23" spans="1:14" ht="32">
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="6" t="s">
         <v>241</v>
       </c>
       <c r="C23" s="21" t="s">
         <v>242</v>
       </c>
-      <c r="D23" s="67" t="s">
+      <c r="D23" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="E23" s="68">
+      <c r="E23" s="8">
         <v>2015</v>
       </c>
       <c r="F23" s="32" t="s">

</xml_diff>

<commit_message>
updated slides and lit. review
</commit_message>
<xml_diff>
--- a/Literature_Review.xlsx
+++ b/Literature_Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/YANG_Chialing/Desktop/Master_Thesis_TUM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83606C18-8012-424A-9744-BA283D47ED46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18E1CEE-A5C8-AC4B-BB80-3BF91E660BF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15820" activeTab="4" xr2:uid="{674E6E98-2842-4292-A448-B304B7BF9135}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="263">
   <si>
     <t>Google Scholar</t>
   </si>
@@ -1051,9 +1051,6 @@
     <t>Madani</t>
   </si>
   <si>
-    <t>RL involved?</t>
-  </si>
-  <si>
     <t>This work</t>
   </si>
   <si>
@@ -1093,13 +1090,25 @@
     <t>Soft Actor-Critic</t>
   </si>
   <si>
-    <t>EV-Aware?</t>
-  </si>
-  <si>
     <t>Metaheuristic: Chaotic-Opposition Based Driving Training-Based Optimization</t>
   </si>
   <si>
     <t>OPF + Unit commitment</t>
+  </si>
+  <si>
+    <t>Network-Constrained Reinforcement Learning for Optimal EV Charging Control</t>
+  </si>
+  <si>
+    <t>Without DC Approximation</t>
+  </si>
+  <si>
+    <t>RL involved</t>
+  </si>
+  <si>
+    <t>EV-Aware</t>
+  </si>
+  <si>
+    <t>2023 IEEE International Conference on Communications, Control, and Computing Technologies for Smart Grids (SmartGridComm)</t>
   </si>
 </sst>
 </file>
@@ -1473,8 +1482,85 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1491,9 +1577,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1509,90 +1592,16 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2968,23 +2977,23 @@
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="40" t="s">
+      <c r="E2" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="52"/>
-      <c r="G2" s="53"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="62"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-      <c r="K2" s="60"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="40" t="s">
+      <c r="M2" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
+      <c r="N2" s="61"/>
+      <c r="O2" s="62"/>
       <c r="P2" s="1"/>
-      <c r="Q2" s="60"/>
+      <c r="Q2" s="64"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -3013,19 +3022,19 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="65"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-      <c r="K3" s="46"/>
+      <c r="K3" s="69"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="59"/>
-      <c r="N3" s="60"/>
-      <c r="O3" s="61"/>
+      <c r="M3" s="63"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="65"/>
       <c r="P3" s="1"/>
-      <c r="Q3" s="46"/>
+      <c r="Q3" s="69"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -3054,19 +3063,19 @@
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="56"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="68"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-      <c r="K4" s="46"/>
+      <c r="K4" s="69"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="54"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="56"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="68"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="46"/>
+      <c r="Q4" s="69"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
@@ -3217,15 +3226,15 @@
       <c r="A8" s="1"/>
       <c r="B8" s="5"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="70" t="s">
         <v>0</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="70" t="s">
         <v>27</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="64" t="s">
+      <c r="H8" s="72" t="s">
         <v>1</v>
       </c>
       <c r="I8" s="4"/>
@@ -3264,11 +3273,11 @@
       <c r="A9" s="1"/>
       <c r="B9" s="5"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="63"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="63"/>
+      <c r="F9" s="71"/>
       <c r="G9" s="4"/>
-      <c r="H9" s="65"/>
+      <c r="H9" s="73"/>
       <c r="I9" s="4"/>
       <c r="J9" s="5"/>
       <c r="K9" s="1"/>
@@ -3391,18 +3400,18 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="47" t="s">
+      <c r="H12" s="79" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="48"/>
-      <c r="J12" s="49"/>
+      <c r="I12" s="80"/>
+      <c r="J12" s="81"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="47" t="s">
+      <c r="M12" s="79" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="50"/>
-      <c r="O12" s="51"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="83"/>
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -3518,18 +3527,18 @@
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
-      <c r="H15" s="47" t="s">
+      <c r="H15" s="79" t="s">
         <v>29</v>
       </c>
-      <c r="I15" s="48"/>
-      <c r="J15" s="49"/>
+      <c r="I15" s="80"/>
+      <c r="J15" s="81"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
-      <c r="M15" s="47" t="s">
+      <c r="M15" s="79" t="s">
         <v>31</v>
       </c>
-      <c r="N15" s="48"/>
-      <c r="O15" s="49"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="81"/>
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
@@ -3645,18 +3654,18 @@
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="40" t="s">
+      <c r="H18" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="I18" s="52"/>
-      <c r="J18" s="53"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="75"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
@@ -3690,14 +3699,14 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
-      <c r="H19" s="54"/>
-      <c r="I19" s="55"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="68"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="44"/>
-      <c r="O19" s="45"/>
+      <c r="M19" s="76"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="78"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
@@ -3813,11 +3822,11 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
-      <c r="H22" s="40" t="s">
+      <c r="H22" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="I22" s="41"/>
-      <c r="J22" s="42"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="75"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -3856,9 +3865,9 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="45"/>
+      <c r="H23" s="76"/>
+      <c r="I23" s="77"/>
+      <c r="J23" s="78"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -3937,10 +3946,10 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="3"/>
-      <c r="G25" s="57" t="s">
+      <c r="G25" s="84" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="58"/>
+      <c r="H25" s="85"/>
       <c r="I25" s="1"/>
       <c r="J25" s="26" t="s">
         <v>19</v>
@@ -4061,8 +4070,8 @@
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
-      <c r="D28" s="46"/>
-      <c r="E28" s="46"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="1"/>
       <c r="G28" s="4"/>
       <c r="H28" s="27"/>
@@ -4592,13 +4601,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E2:G4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="M2:O4"/>
-    <mergeCell ref="Q2:Q4"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="H8:H9"/>
     <mergeCell ref="H22:J23"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="H12:J12"/>
@@ -4608,6 +4610,13 @@
     <mergeCell ref="H18:J19"/>
     <mergeCell ref="M18:O19"/>
     <mergeCell ref="G25:H25"/>
+    <mergeCell ref="E2:G4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="M2:O4"/>
+    <mergeCell ref="Q2:Q4"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="F8:F9"/>
+    <mergeCell ref="H8:H9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -4677,10 +4686,10 @@
         <v>5</v>
       </c>
       <c r="I2" s="7"/>
-      <c r="J2" s="66" t="s">
+      <c r="J2" s="86" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="66"/>
+      <c r="K2" s="86"/>
       <c r="L2" s="7"/>
       <c r="M2" s="7" t="s">
         <v>34</v>
@@ -29214,531 +29223,584 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A75453E-9501-C14B-AE65-E627664C1B87}">
-  <dimension ref="A1:H22"/>
+  <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="46.83203125" style="67" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="67"/>
-    <col min="3" max="3" width="23.1640625" style="67" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" style="67" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" style="67" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" style="67" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" style="67" customWidth="1"/>
-    <col min="8" max="8" width="13.1640625" style="67" customWidth="1"/>
+    <col min="1" max="1" width="46.83203125" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="46.33203125" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="68" t="s">
+    <row r="1" spans="1:9">
+      <c r="A1" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="40" t="s">
         <v>120</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="40" t="s">
+        <v>261</v>
+      </c>
+      <c r="H1" s="40" t="s">
+        <v>260</v>
+      </c>
+      <c r="I1" s="87" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16">
+      <c r="A2" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="D2" s="42">
+        <v>2023</v>
+      </c>
+      <c r="E2" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="G2" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="43"/>
+      <c r="I2" s="47"/>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="45" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="41" t="s">
+        <v>172</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="42">
+        <v>2021</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="F3" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="46"/>
+      <c r="I3" s="47"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="B4" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="42">
+        <v>2012</v>
+      </c>
+      <c r="E4" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="F4" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="G4" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="43"/>
+      <c r="I4" s="47"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="41" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>189</v>
+      </c>
+      <c r="D5" s="42">
+        <v>2021</v>
+      </c>
+      <c r="E5" s="46" t="s">
         <v>257</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="F5" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="G5" s="46"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="47"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="42">
+        <v>2024</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="45" t="s">
+        <v>256</v>
+      </c>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="47"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>212</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>213</v>
+      </c>
+      <c r="D7" s="42">
+        <v>1968</v>
+      </c>
+      <c r="E7" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F7" s="45" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
+      <c r="I7" s="47"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="B8" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="C8" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="42">
+        <v>2000</v>
+      </c>
+      <c r="E8" s="48" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="45" t="s">
+        <v>250</v>
+      </c>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
+      <c r="I8" s="47"/>
+    </row>
+    <row r="9" spans="1:9" ht="16">
+      <c r="A9" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>227</v>
+      </c>
+      <c r="C9" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="42">
+        <v>2017</v>
+      </c>
+      <c r="E9" s="48" t="s">
+        <v>154</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>248</v>
+      </c>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
+      <c r="I9" s="47"/>
+    </row>
+    <row r="10" spans="1:9" ht="16">
+      <c r="A10" s="41" t="s">
+        <v>234</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>235</v>
+      </c>
+      <c r="C10" s="41" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="42">
+        <v>2023</v>
+      </c>
+      <c r="E10" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>249</v>
+      </c>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
+      <c r="I10" s="47"/>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="41" t="s">
+        <v>238</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>239</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="42">
+        <v>2012</v>
+      </c>
+      <c r="E11" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="45" t="s">
+        <v>251</v>
+      </c>
+      <c r="G11" s="48"/>
+      <c r="H11" s="48"/>
+      <c r="I11" s="47"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="41" t="s">
+        <v>241</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>242</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="42">
+        <v>2015</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>121</v>
+      </c>
+      <c r="F12" s="45" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="47"/>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="41" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="42">
+        <v>2020</v>
+      </c>
+      <c r="E13" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" s="45" t="s">
+        <v>252</v>
+      </c>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="47"/>
+    </row>
+    <row r="14" spans="1:9" ht="16">
+      <c r="A14" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="42">
+        <v>2020</v>
+      </c>
+      <c r="E14" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="47"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="42">
+        <v>2021</v>
+      </c>
+      <c r="E15" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="F15" s="41" t="s">
+        <v>244</v>
+      </c>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="47"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="41" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="42">
+        <v>2022</v>
+      </c>
+      <c r="E16" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="F16" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="47"/>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="49" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="50">
+        <v>2022</v>
+      </c>
+      <c r="E17" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F17" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="47"/>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18" s="42">
+        <v>2022</v>
+      </c>
+      <c r="E18" s="43" t="s">
+        <v>141</v>
+      </c>
+      <c r="F18" s="45" t="s">
+        <v>244</v>
+      </c>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="47"/>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D19" s="42">
+        <v>2023</v>
+      </c>
+      <c r="E19" s="43" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" s="45" t="s">
+        <v>255</v>
+      </c>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="47"/>
+    </row>
+    <row r="20" spans="1:9" ht="16">
+      <c r="A20" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="42">
+        <v>2024</v>
+      </c>
+      <c r="E20" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="47"/>
+    </row>
+    <row r="21" spans="1:9" ht="18" customHeight="1">
+      <c r="A21" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="55" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="56">
+        <v>2024</v>
+      </c>
+      <c r="E21" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="47"/>
+    </row>
+    <row r="22" spans="1:9" ht="18" customHeight="1">
+      <c r="A22" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="B22" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C22" s="55" t="s">
+        <v>262</v>
+      </c>
+      <c r="D22" s="56">
+        <v>2023</v>
+      </c>
+      <c r="E22" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="43" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="47"/>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" s="57" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16">
-      <c r="A2" s="69" t="s">
-        <v>164</v>
-      </c>
-      <c r="B2" s="69" t="s">
-        <v>165</v>
-      </c>
-      <c r="C2" s="69" t="s">
-        <v>166</v>
-      </c>
-      <c r="D2" s="70">
-        <v>2023</v>
-      </c>
-      <c r="E2" s="71" t="s">
+      <c r="B23" s="58"/>
+      <c r="C23" s="58"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="54" t="s">
         <v>167</v>
       </c>
-      <c r="F2" s="72" t="s">
-        <v>247</v>
-      </c>
-      <c r="G2" s="71" t="s">
+      <c r="F23" s="53" t="s">
+        <v>244</v>
+      </c>
+      <c r="G23" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="71"/>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="73" t="s">
-        <v>171</v>
-      </c>
-      <c r="B3" s="69" t="s">
-        <v>172</v>
-      </c>
-      <c r="C3" s="73" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="70">
-        <v>2021</v>
-      </c>
-      <c r="E3" s="74" t="s">
-        <v>174</v>
-      </c>
-      <c r="F3" s="73" t="s">
-        <v>170</v>
-      </c>
-      <c r="G3" s="74" t="s">
+      <c r="H23" s="52" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="74"/>
-    </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="69" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="69" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" s="69" t="s">
-        <v>182</v>
-      </c>
-      <c r="D4" s="70">
-        <v>2012</v>
-      </c>
-      <c r="E4" s="71" t="s">
-        <v>167</v>
-      </c>
-      <c r="F4" s="73" t="s">
-        <v>186</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="71"/>
-    </row>
-    <row r="5" spans="1:8">
-      <c r="A5" s="69" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="73" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="D5" s="70">
-        <v>2021</v>
-      </c>
-      <c r="E5" s="74" t="s">
-        <v>259</v>
-      </c>
-      <c r="F5" s="73" t="s">
-        <v>193</v>
-      </c>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="69" t="s">
-        <v>202</v>
-      </c>
-      <c r="B6" s="69" t="s">
-        <v>203</v>
-      </c>
-      <c r="C6" s="73" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="70">
-        <v>2024</v>
-      </c>
-      <c r="E6" s="74" t="s">
-        <v>208</v>
-      </c>
-      <c r="F6" s="73" t="s">
-        <v>258</v>
-      </c>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="75" t="s">
-        <v>211</v>
-      </c>
-      <c r="B7" s="73" t="s">
-        <v>212</v>
-      </c>
-      <c r="C7" s="73" t="s">
-        <v>213</v>
-      </c>
-      <c r="D7" s="70">
-        <v>1968</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>214</v>
-      </c>
-      <c r="F7" s="73" t="s">
-        <v>248</v>
-      </c>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="69" t="s">
-        <v>216</v>
-      </c>
-      <c r="B8" s="73" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="70">
-        <v>2000</v>
-      </c>
-      <c r="E8" s="76" t="s">
-        <v>214</v>
-      </c>
-      <c r="F8" s="73" t="s">
-        <v>251</v>
-      </c>
-      <c r="G8" s="76"/>
-      <c r="H8" s="76"/>
-    </row>
-    <row r="9" spans="1:8" ht="16">
-      <c r="A9" s="75" t="s">
-        <v>226</v>
-      </c>
-      <c r="B9" s="73" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D9" s="70">
-        <v>2017</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>154</v>
-      </c>
-      <c r="F9" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="G9" s="76"/>
-      <c r="H9" s="76"/>
-    </row>
-    <row r="10" spans="1:8" ht="16">
-      <c r="A10" s="69" t="s">
-        <v>234</v>
-      </c>
-      <c r="B10" s="73" t="s">
-        <v>235</v>
-      </c>
-      <c r="C10" s="69" t="s">
-        <v>82</v>
-      </c>
-      <c r="D10" s="70">
-        <v>2023</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="F10" s="72" t="s">
-        <v>250</v>
-      </c>
-      <c r="G10" s="76"/>
-      <c r="H10" s="76"/>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="69" t="s">
-        <v>238</v>
-      </c>
-      <c r="B11" s="73" t="s">
-        <v>239</v>
-      </c>
-      <c r="C11" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D11" s="70">
-        <v>2012</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="F11" s="73" t="s">
-        <v>252</v>
-      </c>
-      <c r="G11" s="76"/>
-      <c r="H11" s="76"/>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="69" t="s">
-        <v>241</v>
-      </c>
-      <c r="B12" s="73" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" s="70">
-        <v>2015</v>
-      </c>
-      <c r="E12" s="76" t="s">
-        <v>121</v>
-      </c>
-      <c r="F12" s="73" t="s">
-        <v>240</v>
-      </c>
-      <c r="G12" s="76"/>
-      <c r="H12" s="76"/>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="69" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="69" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="70">
-        <v>2020</v>
-      </c>
-      <c r="E13" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="F13" s="73" t="s">
-        <v>253</v>
-      </c>
-      <c r="G13" s="71"/>
-      <c r="H13" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16">
-      <c r="A14" s="69" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="D14" s="70">
-        <v>2020</v>
-      </c>
-      <c r="E14" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="72" t="s">
-        <v>254</v>
-      </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="69" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="69" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="70">
-        <v>2021</v>
-      </c>
-      <c r="E15" s="71" t="s">
-        <v>154</v>
-      </c>
-      <c r="F15" s="69" t="s">
-        <v>245</v>
-      </c>
-      <c r="G15" s="71"/>
-      <c r="H15" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="69" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="69" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="69" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" s="70">
-        <v>2022</v>
-      </c>
-      <c r="E16" s="71" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16" s="73" t="s">
-        <v>246</v>
-      </c>
-      <c r="G16" s="71"/>
-      <c r="H16" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="77" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="77" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="77" t="s">
-        <v>59</v>
-      </c>
-      <c r="D17" s="78">
-        <v>2022</v>
-      </c>
-      <c r="E17" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="F17" s="73" t="s">
-        <v>255</v>
-      </c>
-      <c r="G17" s="71"/>
-      <c r="H17" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="69" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="69" t="s">
-        <v>40</v>
-      </c>
-      <c r="C18" s="69" t="s">
-        <v>58</v>
-      </c>
-      <c r="D18" s="70">
-        <v>2022</v>
-      </c>
-      <c r="E18" s="71" t="s">
-        <v>141</v>
-      </c>
-      <c r="F18" s="73" t="s">
-        <v>245</v>
-      </c>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="69" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="69" t="s">
-        <v>56</v>
-      </c>
-      <c r="D19" s="70">
-        <v>2023</v>
-      </c>
-      <c r="E19" s="71" t="s">
-        <v>143</v>
-      </c>
-      <c r="F19" s="73" t="s">
-        <v>256</v>
-      </c>
-      <c r="G19" s="71"/>
-      <c r="H19" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="16">
-      <c r="A20" s="69" t="s">
-        <v>49</v>
-      </c>
-      <c r="B20" s="69" t="s">
-        <v>50</v>
-      </c>
-      <c r="C20" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" s="70">
-        <v>2024</v>
-      </c>
-      <c r="E20" s="71" t="s">
-        <v>121</v>
-      </c>
-      <c r="F20" s="72" t="s">
-        <v>245</v>
-      </c>
-      <c r="G20" s="71"/>
-      <c r="H20" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="18" customHeight="1">
-      <c r="A21" s="83" t="s">
-        <v>51</v>
-      </c>
-      <c r="B21" s="83" t="s">
-        <v>52</v>
-      </c>
-      <c r="C21" s="83" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="84">
-        <v>2024</v>
-      </c>
-      <c r="E21" s="71" t="s">
-        <v>153</v>
-      </c>
-      <c r="F21" s="72" t="s">
-        <v>130</v>
-      </c>
-      <c r="G21" s="71"/>
-      <c r="H21" s="71" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="85" t="s">
-        <v>244</v>
-      </c>
-      <c r="B22" s="86"/>
-      <c r="C22" s="86"/>
-      <c r="D22" s="87"/>
-      <c r="E22" s="82" t="s">
-        <v>167</v>
-      </c>
-      <c r="F22" s="81" t="s">
-        <v>245</v>
-      </c>
-      <c r="G22" s="79" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="80" t="s">
+      <c r="I23" s="51" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>